<commit_message>
added spreadsheet protection to the cells you're not supposed to edit, and marked the ones you are supposed to edit in green
</commit_message>
<xml_diff>
--- a/api-lambda-mock/ec2-vs-lambda.xlsx
+++ b/api-lambda-mock/ec2-vs-lambda.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-17680" yWindow="15040" windowWidth="29700" windowHeight="18580" tabRatio="500"/>
+    <workbookView xWindow="5320" yWindow="10280" windowWidth="29700" windowHeight="18580" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Simple EC2-vs-Lambda" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="102">
   <si>
     <t>AWS EC2 costs for a small SOA architecture</t>
   </si>
@@ -51,9 +51,6 @@
     <t>m3.medium</t>
   </si>
   <si>
-    <t>https://aws.amazon.com/ec2/pricing/</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -286,19 +283,62 @@
   </si>
   <si>
     <t>x ratio (hits)</t>
+  </si>
+  <si>
+    <t>t2.nano</t>
+  </si>
+  <si>
+    <t>t2.micro</t>
+  </si>
+  <si>
+    <t>m4.large</t>
+  </si>
+  <si>
+    <t>m4.xlarge</t>
+  </si>
+  <si>
+    <t>m4.4xlarge</t>
+  </si>
+  <si>
+    <t>m4.10xlarge</t>
+  </si>
+  <si>
+    <t>m3.large</t>
+  </si>
+  <si>
+    <t>m3.2xlarge</t>
+  </si>
+  <si>
+    <t>c3.large</t>
+  </si>
+  <si>
+    <t>c3.xlarge</t>
+  </si>
+  <si>
+    <t>c3.2xlarge</t>
+  </si>
+  <si>
+    <t>c3.4xlarge</t>
+  </si>
+  <si>
+    <t>c3.8xlarge</t>
+  </si>
+  <si>
+    <t>EC2 Server Pricing (us-east-1 / on-demand)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -337,13 +377,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -435,7 +487,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -466,8 +518,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -477,9 +547,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -502,21 +569,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="48">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -532,6 +632,15 @@
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -546,6 +655,15 @@
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -878,7 +996,7 @@
   <dimension ref="B3:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -937,19 +1055,19 @@
         <v>6</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="M5" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11" t="s">
+      <c r="M5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="49"/>
+      <c r="O5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:18">
@@ -957,75 +1075,79 @@
       <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="42">
         <v>3</v>
       </c>
       <c r="F6" s="5">
         <f>IF(F12&lt;$Q$11,E6,CEILING(F12/$Q$11,0)*E6)</f>
         <v>3</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="39">
+        <f>VLOOKUP(D6,$M$12:$N$30,2,FALSE)</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <f>30*24*G6*F6</f>
         <v>144.72</v>
       </c>
       <c r="I6" s="6"/>
-      <c r="M6" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="50"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="4"/>
+      <c r="Q6" s="50"/>
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="E7" s="42">
         <v>3</v>
       </c>
       <c r="F7" s="5">
         <f>IF(F13&lt;$Q$11,E7,CEILING(F13/$Q$11,0)*E7)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="39">
+        <f>VLOOKUP(D7,$M$12:$N$30,2,FALSE)</f>
         <v>0.26600000000000001</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="9">
         <f>30*24*G7*F7</f>
         <v>574.56000000000006</v>
       </c>
       <c r="I7" s="6"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="N7" s="50"/>
       <c r="O7" s="6"/>
-      <c r="P7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>2700000</v>
+      <c r="P7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" s="46">
+        <v>1000000</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="E8" s="42">
         <f>E7*$Q$8</f>
         <v>6</v>
       </c>
@@ -1033,110 +1155,114 @@
         <f>IF(F14&lt;$Q$11,E8,CEILING(F14/$Q$11,0)*E8)</f>
         <v>6</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="39">
+        <f>VLOOKUP(D8,$M$12:$N$30,2,FALSE)</f>
         <v>0.47899999999999998</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <f>30*24*G8*F8</f>
         <v>2069.2799999999997</v>
       </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="4"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="4" t="s">
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="42">
+        <v>8.8739999999999999E-2</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q8" s="42">
+        <v>2</v>
+      </c>
+      <c r="R8" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>2</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="15">
+      <c r="H9" s="12">
         <f>SUM(H6:H8)</f>
         <v>2788.56</v>
       </c>
       <c r="I9" s="6"/>
       <c r="M9" s="4"/>
+      <c r="N9" s="42"/>
       <c r="O9" s="6"/>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q9" s="42">
+        <v>10</v>
+      </c>
+      <c r="R9" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>10</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="4"/>
       <c r="I10" s="6"/>
-      <c r="M10" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="42"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q10" s="33">
+      <c r="P10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q10" s="42">
         <v>10</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="H11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>23</v>
-      </c>
       <c r="I11" s="6"/>
-      <c r="M11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" s="5">
-        <v>8.8739999999999999E-2</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q11" s="5">
+      <c r="M11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="N11" s="42"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q11" s="42">
         <v>1000</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:18">
@@ -1144,170 +1270,219 @@
       <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <f>D13/Q10</f>
-        <v>27000</v>
-      </c>
-      <c r="E12" s="16">
+        <v>10000</v>
+      </c>
+      <c r="E12" s="13">
         <f>D12*$Q$14</f>
-        <v>108000</v>
-      </c>
-      <c r="F12" s="17">
+        <v>40000</v>
+      </c>
+      <c r="F12" s="14">
         <f>D12/24/60/60*($Q$12)</f>
-        <v>6.25</v>
-      </c>
-      <c r="G12" s="16">
+        <v>2.3148148148148149</v>
+      </c>
+      <c r="G12" s="13">
         <f>(E12+D12)*30</f>
-        <v>4050000</v>
-      </c>
-      <c r="H12" s="12">
-        <f>D12*($Q$13/1000)*$N$11</f>
-        <v>2.3959799999999998</v>
+        <v>1500000</v>
+      </c>
+      <c r="H12" s="9">
+        <f>D12*($Q$13/1000)*$N$8</f>
+        <v>0.88739999999999997</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="M12" s="4"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q12" s="5">
+      <c r="M12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" s="43">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q12" s="42">
         <v>20</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="16">
+        <v>10</v>
+      </c>
+      <c r="D13" s="13">
         <f>D14/Q9</f>
-        <v>270000</v>
-      </c>
-      <c r="E13" s="16">
+        <v>100000</v>
+      </c>
+      <c r="E13" s="13">
         <f>D13*$Q$14</f>
-        <v>1080000</v>
-      </c>
-      <c r="F13" s="17">
+        <v>400000</v>
+      </c>
+      <c r="F13" s="14">
         <f>D13/24/60/60*($Q$12)</f>
-        <v>62.5</v>
-      </c>
-      <c r="G13" s="16">
+        <v>23.148148148148149</v>
+      </c>
+      <c r="G13" s="13">
         <f>(E13+D13)*30</f>
-        <v>40500000</v>
-      </c>
-      <c r="H13" s="12">
-        <f>D13*($Q$13/1000)*$N$11</f>
-        <v>23.959800000000001</v>
+        <v>15000000</v>
+      </c>
+      <c r="H13" s="9">
+        <f>D13*($Q$13/1000)*$N$8</f>
+        <v>8.8740000000000006</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="M13" s="4"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q13" s="5">
+      <c r="M13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" s="43">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" s="42">
         <v>1</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="16">
+        <v>12</v>
+      </c>
+      <c r="D14" s="13">
         <f>Q7</f>
-        <v>2700000</v>
-      </c>
-      <c r="E14" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="E14" s="13">
         <f>D14*$Q$14</f>
-        <v>10800000</v>
-      </c>
-      <c r="F14" s="17">
+        <v>4000000</v>
+      </c>
+      <c r="F14" s="14">
         <f>D14/24/60/60*($Q$12)</f>
-        <v>625</v>
-      </c>
-      <c r="G14" s="16">
+        <v>231.4814814814815</v>
+      </c>
+      <c r="G14" s="13">
         <f>(E14+D14)*30</f>
-        <v>405000000</v>
-      </c>
-      <c r="H14" s="12">
-        <f>D14*($Q$13/1000)*$N$11</f>
-        <v>239.59799999999998</v>
+        <v>150000000</v>
+      </c>
+      <c r="H14" s="9">
+        <f>D14*($Q$13/1000)*$N$8</f>
+        <v>88.74</v>
       </c>
       <c r="I14" s="6"/>
-      <c r="M14" s="4"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q14" s="33">
+      <c r="M14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="43">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q14" s="42">
         <v>4</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="19">
+      <c r="H15" s="16">
         <f>SUM(H12:H14)</f>
-        <v>265.95377999999999</v>
+        <v>98.50139999999999</v>
       </c>
       <c r="I15" s="6"/>
-      <c r="M15" s="4"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="4"/>
+      <c r="M15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="43">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="42"/>
       <c r="R15" s="6"/>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="4"/>
       <c r="I16" s="6"/>
-      <c r="M16" s="4"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="43">
+        <v>0.104</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="42"/>
       <c r="R16" s="6"/>
     </row>
     <row r="17" spans="2:18" s="8" customFormat="1">
-      <c r="B17" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22">
+      <c r="B17" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19">
         <f>H15+H9</f>
-        <v>3054.5137799999998</v>
-      </c>
-      <c r="I17" s="23"/>
-      <c r="M17" s="7"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="7"/>
-      <c r="R17" s="36"/>
+        <v>2887.0614</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="M17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N17" s="43">
+        <v>0.12</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="32"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="M18" s="4"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="4"/>
+      <c r="M18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18" s="43">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="42"/>
       <c r="R18" s="6"/>
     </row>
     <row r="19" spans="2:18" s="8" customFormat="1">
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1318,17 +1493,31 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="3"/>
-      <c r="M19" s="7"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="7"/>
-      <c r="R19" s="36"/>
+      <c r="M19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N19" s="43">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="32"/>
     </row>
     <row r="20" spans="2:18">
       <c r="B20" s="4"/>
       <c r="K20" s="6"/>
-      <c r="M20" s="4"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N20" s="43">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="42"/>
       <c r="R20" s="6"/>
     </row>
     <row r="21" spans="2:18">
@@ -1340,7 +1529,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
@@ -1350,9 +1539,16 @@
         <v>6</v>
       </c>
       <c r="K21" s="6"/>
-      <c r="M21" s="4"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="4"/>
+      <c r="M21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N21" s="43">
+        <v>2.3940000000000001</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="42"/>
       <c r="R21" s="6"/>
     </row>
     <row r="22" spans="2:18">
@@ -1360,101 +1556,139 @@
       <c r="C22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="24">
+      <c r="D22" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="41">
         <v>2</v>
       </c>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24">
+      <c r="F22" s="21"/>
+      <c r="G22" s="39">
+        <f>VLOOKUP(D22,$M$12:$N$30,2,FALSE)</f>
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="9">
         <f>30*24*G22*E22</f>
         <v>37.44</v>
       </c>
       <c r="K22" s="6"/>
-      <c r="M22" s="4"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="4"/>
+      <c r="M22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" s="43">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="42"/>
       <c r="R22" s="6"/>
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="4"/>
       <c r="C23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="24">
+        <v>10</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="41">
         <v>2</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24">
+      <c r="F23" s="21"/>
+      <c r="G23" s="39">
+        <f>VLOOKUP(D23,$M$12:$N$30,2,FALSE)</f>
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="9">
         <f>30*24*G23*E23</f>
         <v>74.88</v>
       </c>
       <c r="K23" s="6"/>
-      <c r="M23" s="4"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="4"/>
+      <c r="M23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N23" s="43">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="42"/>
       <c r="R23" s="6"/>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="24">
+        <v>12</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="41">
         <v>2</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24">
+      <c r="F24" s="21"/>
+      <c r="G24" s="39">
+        <f>VLOOKUP(D24,$M$12:$N$30,2,FALSE)</f>
         <v>0.104</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="9">
         <f>30*24*G24*E24</f>
         <v>149.76</v>
       </c>
       <c r="K24" s="6"/>
-      <c r="M24" s="4"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="43">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="42"/>
       <c r="R24" s="6"/>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="15">
+      <c r="H25" s="12">
         <f>SUM(H22:H24)</f>
         <v>262.08</v>
       </c>
       <c r="K25" s="6"/>
-      <c r="M25" s="4"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="4"/>
+      <c r="M25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N25" s="43">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="42"/>
       <c r="R25" s="6"/>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="4"/>
       <c r="K26" s="6"/>
-      <c r="M26" s="4"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="4"/>
+      <c r="M26" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="N26" s="44">
+        <v>0.105</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="42"/>
       <c r="R26" s="6"/>
     </row>
     <row r="27" spans="2:18">
@@ -1482,17 +1716,23 @@
       </c>
       <c r="I27" s="8"/>
       <c r="K27" s="6"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="4" t="s">
+      <c r="M27" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="N27" s="44">
+        <v>0.21</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q27" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="R27" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="Q27" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="R27" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:18">
@@ -1501,27 +1741,34 @@
         <f t="shared" ref="C28:D30" si="1">C12</f>
         <v>dev</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="13">
         <f t="shared" si="1"/>
-        <v>27000</v>
-      </c>
-      <c r="E28" s="16">
+        <v>10000</v>
+      </c>
+      <c r="E28" s="13">
         <f>E12*$Q$27</f>
-        <v>270000</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16">
+        <v>100000</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13">
         <f>(E28+D28)*30</f>
-        <v>8910000</v>
-      </c>
-      <c r="H28" s="12">
-        <f>D28*($Q$13/1000)*$N$11</f>
-        <v>2.3959799999999998</v>
+        <v>3300000</v>
+      </c>
+      <c r="H28" s="9">
+        <f>D28*($Q$13/1000)*$N$8</f>
+        <v>0.88739999999999997</v>
       </c>
       <c r="K28" s="6"/>
-      <c r="M28" s="4"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="4"/>
+      <c r="M28" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="N28" s="44">
+        <v>0.42</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="42"/>
       <c r="R28" s="6"/>
     </row>
     <row r="29" spans="2:18">
@@ -1530,27 +1777,34 @@
         <f t="shared" si="1"/>
         <v>test</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="13">
         <f t="shared" si="1"/>
-        <v>270000</v>
-      </c>
-      <c r="E29" s="16">
+        <v>100000</v>
+      </c>
+      <c r="E29" s="13">
         <f>E13*$Q$27</f>
-        <v>2700000</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13">
         <f>(E29+D29)*30</f>
-        <v>89100000</v>
-      </c>
-      <c r="H29" s="12">
-        <f>D29*($Q$13/1000)*$N$11</f>
-        <v>23.959800000000001</v>
+        <v>33000000</v>
+      </c>
+      <c r="H29" s="9">
+        <f>D29*($Q$13/1000)*$N$8</f>
+        <v>8.8740000000000006</v>
       </c>
       <c r="K29" s="6"/>
-      <c r="M29" s="4"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="4"/>
+      <c r="M29" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="N29" s="44">
+        <v>0.84</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q29" s="42"/>
       <c r="R29" s="6"/>
     </row>
     <row r="30" spans="2:18">
@@ -1559,27 +1813,34 @@
         <f t="shared" si="1"/>
         <v>prod</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="13">
         <f t="shared" si="1"/>
-        <v>2700000</v>
-      </c>
-      <c r="E30" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="E30" s="13">
         <f>E14*$Q$27</f>
-        <v>27000000</v>
-      </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16">
+        <v>10000000</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13">
         <f>(E30+D30)*30</f>
-        <v>891000000</v>
-      </c>
-      <c r="H30" s="12">
-        <f>D30*($Q$13/1000)*$N$11</f>
-        <v>239.59799999999998</v>
+        <v>330000000</v>
+      </c>
+      <c r="H30" s="9">
+        <f>D30*($Q$13/1000)*$N$8</f>
+        <v>88.74</v>
       </c>
       <c r="K30" s="6"/>
-      <c r="M30" s="4"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="4"/>
+      <c r="M30" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="N30" s="44">
+        <v>1.68</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q30" s="42"/>
       <c r="R30" s="6"/>
     </row>
     <row r="31" spans="2:18">
@@ -1592,69 +1853,71 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="26">
+      <c r="H31" s="23">
         <f t="shared" si="2"/>
-        <v>265.95377999999999</v>
+        <v>98.50139999999999</v>
       </c>
       <c r="K31" s="6"/>
       <c r="M31" s="4"/>
+      <c r="N31" s="42"/>
       <c r="O31" s="6"/>
-      <c r="P31" s="4"/>
+      <c r="Q31" s="42"/>
       <c r="R31" s="6"/>
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="4"/>
       <c r="K32" s="6"/>
       <c r="M32" s="7" t="s">
-        <v>84</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="N32" s="42"/>
       <c r="O32" s="6"/>
-      <c r="P32" s="4"/>
+      <c r="Q32" s="42"/>
       <c r="R32" s="6"/>
     </row>
     <row r="33" spans="2:18">
       <c r="B33" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="J33" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J33" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K33" s="36"/>
+      <c r="K33" s="32"/>
       <c r="L33" s="8"/>
       <c r="M33" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N33" s="12">
+        <v>36</v>
+      </c>
+      <c r="N33" s="45">
         <v>0.2</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q33" s="42">
+        <v>100</v>
+      </c>
+      <c r="R33" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="Q33" s="5">
-        <v>100</v>
-      </c>
-      <c r="R33" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:18">
@@ -1663,50 +1926,50 @@
         <f>C28</f>
         <v>dev</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="13">
         <f t="shared" ref="D34" si="3">D28</f>
-        <v>27000</v>
-      </c>
-      <c r="E34" s="16">
+        <v>10000</v>
+      </c>
+      <c r="E34" s="13">
         <f>E28</f>
-        <v>270000</v>
-      </c>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16">
+        <v>100000</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13">
         <f>30*(E34+D34)</f>
-        <v>8910000</v>
-      </c>
-      <c r="H34" s="16">
+        <v>3300000</v>
+      </c>
+      <c r="H34" s="13">
         <f>((D34+(E34*(1-$Q$35)))*30*($Q$33/1000)*($Q$34/1000))+((E34*$Q$35)*30*($Q$36/1000)*($Q$37/1000))</f>
-        <v>2166912</v>
-      </c>
-      <c r="I34" s="12">
+        <v>802560</v>
+      </c>
+      <c r="I34" s="9">
         <f>(G34/1000000)*$N$33</f>
-        <v>1.782</v>
-      </c>
-      <c r="J34" s="27">
+        <v>0.66</v>
+      </c>
+      <c r="J34" s="24">
         <f>H34*$N$34</f>
-        <v>36.122423040000001</v>
-      </c>
-      <c r="K34" s="40"/>
-      <c r="L34" s="27"/>
+        <v>13.378675200000002</v>
+      </c>
+      <c r="K34" s="35"/>
+      <c r="L34" s="24"/>
       <c r="M34" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N34" s="5">
+        <v>62</v>
+      </c>
+      <c r="N34" s="42">
         <v>1.6670000000000001E-5</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q34" s="42">
+        <v>192</v>
+      </c>
+      <c r="R34" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="Q34" s="5">
-        <v>192</v>
-      </c>
-      <c r="R34" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="35" spans="2:18">
@@ -1715,50 +1978,50 @@
         <f t="shared" ref="C35:D36" si="4">C29</f>
         <v>test</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="13">
         <f t="shared" si="4"/>
-        <v>270000</v>
-      </c>
-      <c r="E35" s="16">
+        <v>100000</v>
+      </c>
+      <c r="E35" s="13">
         <f>E29</f>
-        <v>2700000</v>
-      </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13">
         <f>30*(E35+D35)</f>
-        <v>89100000</v>
-      </c>
-      <c r="H35" s="16">
+        <v>33000000</v>
+      </c>
+      <c r="H35" s="13">
         <f>((D35+(E35*(1-$Q$35)))*30*($Q$33/1000)*($Q$34/1000))+((E35*$Q$35)*30*($Q$36/1000)*($Q$37/1000))</f>
-        <v>21669120</v>
-      </c>
-      <c r="I35" s="12">
+        <v>8025600</v>
+      </c>
+      <c r="I35" s="9">
         <f>(G35/1000000)*$N$33</f>
-        <v>17.82</v>
-      </c>
-      <c r="J35" s="27">
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="J35" s="24">
         <f>H35*$N$34</f>
-        <v>361.22423040000001</v>
-      </c>
-      <c r="K35" s="40"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="28" t="s">
+        <v>133.78675200000001</v>
+      </c>
+      <c r="K35" s="35"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="N35" s="46">
+        <v>1000000</v>
+      </c>
+      <c r="O35" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="N35" s="16">
-        <v>1000000</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="P35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q35" s="5">
+      <c r="P35" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q35" s="42">
         <v>0.5</v>
       </c>
       <c r="R35" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:18">
@@ -1767,173 +2030,175 @@
         <f t="shared" si="4"/>
         <v>prod</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="13">
         <f t="shared" si="4"/>
-        <v>2700000</v>
-      </c>
-      <c r="E36" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="E36" s="13">
         <f>E30</f>
-        <v>27000000</v>
-      </c>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16">
+        <v>10000000</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13">
         <f>30*(E36+D36)</f>
-        <v>891000000</v>
-      </c>
-      <c r="H36" s="16">
+        <v>330000000</v>
+      </c>
+      <c r="H36" s="13">
         <f>((D36+(E36*(1-$Q$35)))*30*($Q$33/1000)*($Q$34/1000))+((E36*$Q$35)*30*($Q$36/1000)*($Q$37/1000))</f>
-        <v>216691200</v>
-      </c>
-      <c r="I36" s="12">
+        <v>80256000</v>
+      </c>
+      <c r="I36" s="9">
         <f>(G36/1000000)*$N$33</f>
-        <v>178.20000000000002</v>
-      </c>
-      <c r="J36" s="27">
+        <v>66</v>
+      </c>
+      <c r="J36" s="24">
         <f>H36*$N$34</f>
-        <v>3612.2423040000003</v>
-      </c>
-      <c r="K36" s="40"/>
-      <c r="L36" s="27"/>
+        <v>1337.86752</v>
+      </c>
+      <c r="K36" s="35"/>
+      <c r="L36" s="24"/>
       <c r="M36" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N36" s="16">
+        <v>38</v>
+      </c>
+      <c r="N36" s="46">
         <v>1600000</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="P36" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q36" s="33">
+        <v>66</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q36" s="42">
         <v>1000</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:18">
       <c r="B37" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16">
+        <v>39</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13">
         <f>SUM(G34:G36)</f>
-        <v>989010000</v>
-      </c>
-      <c r="H37" s="16">
+        <v>366300000</v>
+      </c>
+      <c r="H37" s="13">
         <f>SUM(H34:H36)</f>
-        <v>240527232</v>
-      </c>
-      <c r="I37" s="12">
+        <v>89084160</v>
+      </c>
+      <c r="I37" s="9">
         <f>(G37/1000000)*$N$33</f>
-        <v>197.80200000000002</v>
-      </c>
-      <c r="J37" s="27">
+        <v>73.260000000000005</v>
+      </c>
+      <c r="J37" s="24">
         <f>H37*$N$34</f>
-        <v>4009.5889574400003</v>
-      </c>
-      <c r="K37" s="40"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="16"/>
+        <v>1485.0329472000001</v>
+      </c>
+      <c r="K37" s="35"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="46"/>
       <c r="O37" s="6"/>
-      <c r="P37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q37" s="33">
+      <c r="P37" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q37" s="42">
         <v>512</v>
       </c>
       <c r="R37" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="2:18">
       <c r="B38" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30">
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27">
         <f>IF(G37&gt;N35,G37-N35,0)</f>
-        <v>988010000</v>
-      </c>
-      <c r="H38" s="30">
+        <v>365300000</v>
+      </c>
+      <c r="H38" s="27">
         <f>IF(H37&gt;N36,H37-N36,0)</f>
-        <v>238927232</v>
-      </c>
-      <c r="I38" s="15">
+        <v>87484160</v>
+      </c>
+      <c r="I38" s="12">
         <f>(G38/1000000)*$N$33</f>
-        <v>197.602</v>
-      </c>
-      <c r="J38" s="26">
+        <v>73.06</v>
+      </c>
+      <c r="J38" s="23">
         <f>H38*$N$34</f>
-        <v>3982.9169574400003</v>
-      </c>
-      <c r="K38" s="41"/>
-      <c r="L38" s="26"/>
+        <v>1458.3609472000001</v>
+      </c>
+      <c r="K38" s="36"/>
+      <c r="L38" s="23"/>
       <c r="M38" s="4"/>
+      <c r="N38" s="42"/>
       <c r="O38" s="6"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="34"/>
+      <c r="P38" s="38"/>
+      <c r="Q38" s="48"/>
       <c r="R38" s="6"/>
     </row>
     <row r="39" spans="2:18">
       <c r="B39" s="4"/>
       <c r="K39" s="6"/>
       <c r="M39" s="7" t="s">
-        <v>83</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="N39" s="42"/>
       <c r="O39" s="6"/>
-      <c r="P39" s="4"/>
+      <c r="Q39" s="42"/>
       <c r="R39" s="6"/>
     </row>
     <row r="40" spans="2:18">
       <c r="B40" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="31" t="s">
+      <c r="I40" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="I40" s="31" t="s">
+      <c r="J40" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="J40" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="K40" s="42"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="N40" s="5">
+      <c r="K40" s="37"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="N40" s="42">
         <v>1.4E-2</v>
       </c>
-      <c r="O40" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="P40" s="4" t="s">
+      <c r="O40" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q40" s="42">
+        <v>10</v>
+      </c>
+      <c r="R40" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="Q40" s="33">
-        <v>10</v>
-      </c>
-      <c r="R40" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="41" spans="2:18">
@@ -1942,39 +2207,39 @@
         <f>C34</f>
         <v>dev</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="22">
         <f>E34+D34</f>
-        <v>297000</v>
-      </c>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25">
+        <v>110000</v>
+      </c>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22">
         <f>E41*30</f>
-        <v>8910000</v>
+        <v>3300000</v>
       </c>
       <c r="H41" s="5">
         <f>IF(E41 &lt;(24*60*60)*1000,24,E41/60/60/1000)*$Q$40</f>
         <v>240</v>
       </c>
-      <c r="I41" s="27">
+      <c r="I41" s="24">
         <f>G41/100000*$N$40*($Q$13/$N$42)</f>
-        <v>4.9895999999999994</v>
-      </c>
-      <c r="J41" s="27">
+        <v>1.8480000000000001</v>
+      </c>
+      <c r="J41" s="24">
         <f>H41*$N$41*30</f>
         <v>107.99999999999999</v>
       </c>
-      <c r="K41" s="40"/>
-      <c r="L41" s="27"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="24"/>
       <c r="M41" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="N41" s="5">
+        <v>47</v>
+      </c>
+      <c r="N41" s="42">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P41" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="Q41" s="42"/>
       <c r="R41" s="6"/>
     </row>
     <row r="42" spans="2:18">
@@ -1983,40 +2248,39 @@
         <f t="shared" ref="C42:C43" si="5">C35</f>
         <v>test</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="22">
         <f>E35+D35</f>
-        <v>2970000</v>
-      </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25">
+        <v>1100000</v>
+      </c>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22">
         <f>E42*30</f>
-        <v>89100000</v>
+        <v>33000000</v>
       </c>
       <c r="H42" s="5">
         <f>IF(E42 &lt;(24*60*60)*1000,24,E42/60/60/1000)*$Q$40</f>
         <v>240</v>
       </c>
-      <c r="I42" s="27">
+      <c r="I42" s="24">
         <f>G42/100000*$N$40*($Q$13/$N$42)</f>
-        <v>49.896000000000001</v>
-      </c>
-      <c r="J42" s="27">
+        <v>18.48</v>
+      </c>
+      <c r="J42" s="24">
         <f>H42*$N$41*30</f>
         <v>107.99999999999999</v>
       </c>
-      <c r="K42" s="40"/>
-      <c r="L42" s="27"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="24"/>
       <c r="M42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="N42" s="5">
+        <v>85</v>
+      </c>
+      <c r="N42" s="42">
         <v>0.25</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="34"/>
+        <v>70</v>
+      </c>
+      <c r="Q42" s="48"/>
       <c r="R42" s="6"/>
     </row>
     <row r="43" spans="2:18">
@@ -2025,37 +2289,38 @@
         <f t="shared" si="5"/>
         <v>prod</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="22">
         <f>E36+D36</f>
-        <v>29700000</v>
-      </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25">
+        <v>11000000</v>
+      </c>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22">
         <f>E43*30</f>
-        <v>891000000</v>
+        <v>330000000</v>
       </c>
       <c r="H43" s="5">
         <f>IF(E43 &lt;(24*60*60)*1000,24,E43/60/60/1000)*$Q$40</f>
         <v>240</v>
       </c>
-      <c r="I43" s="27">
+      <c r="I43" s="24">
         <f>G43/100000*$N$40*($Q$13/$N$42)</f>
-        <v>498.96000000000004</v>
-      </c>
-      <c r="J43" s="27">
+        <v>184.8</v>
+      </c>
+      <c r="J43" s="24">
         <f>H43*$N$41*30</f>
         <v>107.99999999999999</v>
       </c>
-      <c r="K43" s="40"/>
-      <c r="L43" s="27"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="24"/>
       <c r="M43" s="4"/>
+      <c r="N43" s="50"/>
       <c r="O43" s="6"/>
-      <c r="P43" s="4"/>
+      <c r="Q43" s="50"/>
       <c r="R43" s="6"/>
     </row>
     <row r="44" spans="2:18">
       <c r="B44" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -2063,56 +2328,56 @@
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
-      <c r="I44" s="26">
+      <c r="I44" s="23">
         <f>SUM(I41:I43)</f>
-        <v>553.84559999999999</v>
-      </c>
-      <c r="J44" s="26">
+        <v>205.12800000000001</v>
+      </c>
+      <c r="J44" s="23">
         <f>SUM(J41:J43)</f>
         <v>323.99999999999994</v>
       </c>
-      <c r="K44" s="41"/>
-      <c r="L44" s="26"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="23"/>
       <c r="M44" s="4"/>
+      <c r="N44" s="50"/>
       <c r="O44" s="6"/>
-      <c r="P44" s="4"/>
+      <c r="Q44" s="50"/>
       <c r="R44" s="6"/>
     </row>
     <row r="45" spans="2:18">
       <c r="B45" s="4"/>
       <c r="K45" s="6"/>
-      <c r="M45" s="4"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="13"/>
-      <c r="R45" s="14"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="51"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="51"/>
+      <c r="R45" s="11"/>
     </row>
     <row r="46" spans="2:18" s="8" customFormat="1">
-      <c r="B46" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="32">
+      <c r="B46" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="29">
         <f>I38+J38+H31+H25+I44+J44</f>
-        <v>5586.3983374399995</v>
-      </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="23"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="21"/>
-      <c r="O46" s="23"/>
+        <v>2421.1303472</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="20"/>
     </row>
     <row r="49" spans="2:2" s="8" customFormat="1">
       <c r="B49" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
fix a bug in the upscaling for traditional
</commit_message>
<xml_diff>
--- a/api-lambda-mock/ec2-vs-lambda.xlsx
+++ b/api-lambda-mock/ec2-vs-lambda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="10280" windowWidth="29700" windowHeight="18580" tabRatio="500"/>
+    <workbookView xWindow="5320" yWindow="10280" windowWidth="29700" windowHeight="19860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Simple EC2-vs-Lambda" sheetId="1" r:id="rId1"/>
@@ -530,9 +530,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -664,7 +666,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="50">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -689,6 +691,7 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -712,6 +715,7 @@
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1044,7 +1048,7 @@
   <dimension ref="B2:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1139,7 +1143,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="5">
-        <f>IF(F12&lt;$Q$11,E6,CEILING(F12/$Q$11,0)*E6)</f>
+        <f>IF(F12&lt;$Q$11,E6,ROUND(F12/$Q$11,0)*E6)</f>
         <v>3</v>
       </c>
       <c r="G6" s="39">
@@ -1169,7 +1173,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="5">
-        <f>IF(F13&lt;$Q$11,E7,CEILING(F13/$Q$11,0)*E7)</f>
+        <f>IF(F13&lt;$Q$11,E7,ROUND(F13/$Q$11,0)*E7)</f>
         <v>3</v>
       </c>
       <c r="G7" s="39">
@@ -1209,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="5">
-        <f>IF(F14&lt;$Q$11,E8,CEILING(F14/$Q$11,0)*E8)</f>
+        <f>IF(F14&lt;$Q$11,E8,ROUND(F14/$Q$11,0)*E8)</f>
         <v>6</v>
       </c>
       <c r="G8" s="39">

</xml_diff>

<commit_message>
Add the ec2 comparison for Ithaka
</commit_message>
<xml_diff>
--- a/api-lambda-mock/ec2-vs-lambda.xlsx
+++ b/api-lambda-mock/ec2-vs-lambda.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="10280" windowWidth="29700" windowHeight="19860" tabRatio="500"/>
+    <workbookView xWindow="13600" yWindow="7780" windowWidth="35480" windowHeight="30920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple EC2-vs-Lambda" sheetId="1" r:id="rId1"/>
+    <sheet name="Complex EC2-vs-Lambda )" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,8 +19,120 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Barry A Dobyns</author>
+  </authors>
+  <commentList>
+    <comment ref="D31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Barry A Dobyns:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphite.acorn.cirrostratus.org
+Captain's Log Eventtypes
+24*4*(Views | Downloads | Unauth - last seven days)
++ 24*7*(Sessions)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Barry A Dobyns:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+actual numbers pulled from app dynamics</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Barry A Dobyns:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphite.acorn.cirrostratus.org
+Captain's Log Eventtypes
+24*4*(Views | Downloads | Unauth - last seven days)
++ 24*7*(Sessions)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Barry A Dobyns:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+actual numbers pulled from app dynamics</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="122">
   <si>
     <t>AWS EC2 costs for a small SOA architecture</t>
   </si>
@@ -331,6 +444,60 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>AWS EC2 costs for a very complicated SOA architecture</t>
+  </si>
+  <si>
+    <t>c1.medium</t>
+  </si>
+  <si>
+    <t>g2.2xlarge</t>
+  </si>
+  <si>
+    <t>hi1.4xlarge</t>
+  </si>
+  <si>
+    <t>m1.large</t>
+  </si>
+  <si>
+    <t>m1.xlarge</t>
+  </si>
+  <si>
+    <t>m1.medium</t>
+  </si>
+  <si>
+    <t>m1.small</t>
+  </si>
+  <si>
+    <t>m2.4xlarge</t>
+  </si>
+  <si>
+    <t>c4.4xlarge</t>
+  </si>
+  <si>
+    <t>subtotal test</t>
+  </si>
+  <si>
+    <t>subtotal prod</t>
+  </si>
+  <si>
+    <t>YOU DON'T REALLY WANT TO EDIT PRICING</t>
+  </si>
+  <si>
+    <t>BECAUSE IT'S SET BY AWS/AZURE/WHOEVER</t>
+  </si>
+  <si>
+    <t>med %</t>
+  </si>
+  <si>
+    <t>med calls</t>
+  </si>
+  <si>
+    <t>med mem</t>
+  </si>
+  <si>
+    <t>mid medium/light</t>
   </si>
 </sst>
 </file>
@@ -344,7 +511,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -388,6 +555,19 @@
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -530,7 +710,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -581,8 +761,80 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -665,8 +917,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="122">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -692,6 +950,42 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -716,6 +1010,42 @@
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1047,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1320,7 +1650,7 @@
         <v>57</v>
       </c>
       <c r="Q11" s="42">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="R11" s="6" t="s">
         <v>14</v>
@@ -1341,7 +1671,7 @@
       </c>
       <c r="F12" s="14">
         <f>D12/24/60/60*($Q$12)</f>
-        <v>2.3148148148148149</v>
+        <v>3.3564814814814814</v>
       </c>
       <c r="G12" s="13">
         <f>(E12+D12)*30</f>
@@ -1365,7 +1695,7 @@
         <v>58</v>
       </c>
       <c r="Q12" s="42">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="R12" s="6" t="s">
         <v>87</v>
@@ -1386,7 +1716,7 @@
       </c>
       <c r="F13" s="14">
         <f>D13/24/60/60*($Q$12)</f>
-        <v>23.148148148148149</v>
+        <v>33.564814814814817</v>
       </c>
       <c r="G13" s="13">
         <f>(E13+D13)*30</f>
@@ -1431,7 +1761,7 @@
       </c>
       <c r="F14" s="14">
         <f>D14/24/60/60*($Q$12)</f>
-        <v>231.4814814814815</v>
+        <v>335.64814814814815</v>
       </c>
       <c r="G14" s="13">
         <f>(E14+D14)*30</f>
@@ -1790,7 +2120,7 @@
         <v>60</v>
       </c>
       <c r="Q27" s="42">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="R27" s="6" t="s">
         <v>61</v>
@@ -1808,12 +2138,12 @@
       </c>
       <c r="E28" s="13">
         <f>E12*$Q$27</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="13">
         <f>(E28+D28)*30</f>
-        <v>3300000</v>
+        <v>6300000</v>
       </c>
       <c r="H28" s="9">
         <f>D28*($Q$13/1000)*$N$8</f>
@@ -1844,12 +2174,12 @@
       </c>
       <c r="E29" s="13">
         <f>E13*$Q$27</f>
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="13">
         <f>(E29+D29)*30</f>
-        <v>33000000</v>
+        <v>63000000</v>
       </c>
       <c r="H29" s="9">
         <f>D29*($Q$13/1000)*$N$8</f>
@@ -1880,12 +2210,12 @@
       </c>
       <c r="E30" s="13">
         <f>E14*$Q$27</f>
-        <v>10000000</v>
+        <v>20000000</v>
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="13">
         <f>(E30+D30)*30</f>
-        <v>330000000</v>
+        <v>630000000</v>
       </c>
       <c r="H30" s="9">
         <f>D30*($Q$13/1000)*$N$8</f>
@@ -1993,24 +2323,24 @@
       </c>
       <c r="E34" s="13">
         <f>E28</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13">
         <f>30*(E34+D34)</f>
-        <v>3300000</v>
+        <v>6300000</v>
       </c>
       <c r="H34" s="13">
         <f>((D34+(E34*(1-$Q$35)))*30*($Q$33/1000)*($Q$34/1000))+((E34*$Q$35)*30*($Q$36/1000)*($Q$37/1000))</f>
-        <v>802560</v>
+        <v>1599360</v>
       </c>
       <c r="I34" s="9">
         <f>(G34/1000000)*$N$33</f>
-        <v>0.66</v>
+        <v>1.26</v>
       </c>
       <c r="J34" s="24">
         <f>H34*$N$34</f>
-        <v>13.378675200000002</v>
+        <v>26.661331200000003</v>
       </c>
       <c r="K34" s="35"/>
       <c r="L34" s="24"/>
@@ -2045,24 +2375,24 @@
       </c>
       <c r="E35" s="13">
         <f>E29</f>
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="F35" s="13"/>
       <c r="G35" s="13">
         <f>30*(E35+D35)</f>
-        <v>33000000</v>
+        <v>63000000</v>
       </c>
       <c r="H35" s="13">
         <f>((D35+(E35*(1-$Q$35)))*30*($Q$33/1000)*($Q$34/1000))+((E35*$Q$35)*30*($Q$36/1000)*($Q$37/1000))</f>
-        <v>8025600</v>
+        <v>15993600</v>
       </c>
       <c r="I35" s="9">
         <f>(G35/1000000)*$N$33</f>
-        <v>6.6000000000000005</v>
+        <v>12.600000000000001</v>
       </c>
       <c r="J35" s="24">
         <f>H35*$N$34</f>
-        <v>133.78675200000001</v>
+        <v>266.61331200000001</v>
       </c>
       <c r="K35" s="35"/>
       <c r="L35" s="24"/>
@@ -2097,24 +2427,24 @@
       </c>
       <c r="E36" s="13">
         <f>E30</f>
-        <v>10000000</v>
+        <v>20000000</v>
       </c>
       <c r="F36" s="13"/>
       <c r="G36" s="13">
         <f>30*(E36+D36)</f>
-        <v>330000000</v>
+        <v>630000000</v>
       </c>
       <c r="H36" s="13">
         <f>((D36+(E36*(1-$Q$35)))*30*($Q$33/1000)*($Q$34/1000))+((E36*$Q$35)*30*($Q$36/1000)*($Q$37/1000))</f>
-        <v>80256000</v>
+        <v>159936000</v>
       </c>
       <c r="I36" s="9">
         <f>(G36/1000000)*$N$33</f>
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="J36" s="24">
         <f>H36*$N$34</f>
-        <v>1337.86752</v>
+        <v>2666.1331200000004</v>
       </c>
       <c r="K36" s="35"/>
       <c r="L36" s="24"/>
@@ -2146,19 +2476,19 @@
       <c r="F37" s="13"/>
       <c r="G37" s="13">
         <f>SUM(G34:G36)</f>
-        <v>366300000</v>
+        <v>699300000</v>
       </c>
       <c r="H37" s="13">
         <f>SUM(H34:H36)</f>
-        <v>89084160</v>
+        <v>177528960</v>
       </c>
       <c r="I37" s="9">
         <f>(G37/1000000)*$N$33</f>
-        <v>73.260000000000005</v>
+        <v>139.85999999999999</v>
       </c>
       <c r="J37" s="24">
         <f>H37*$N$34</f>
-        <v>1485.0329472000001</v>
+        <v>2959.4077632000003</v>
       </c>
       <c r="K37" s="35"/>
       <c r="L37" s="24"/>
@@ -2185,19 +2515,19 @@
       <c r="F38" s="27"/>
       <c r="G38" s="27">
         <f>IF(G37&gt;N35,G37-N35,0)</f>
-        <v>365300000</v>
+        <v>698300000</v>
       </c>
       <c r="H38" s="27">
         <f>IF(H37&gt;N36,H37-N36,0)</f>
-        <v>87484160</v>
+        <v>175928960</v>
       </c>
       <c r="I38" s="12">
         <f>(G38/1000000)*$N$33</f>
-        <v>73.06</v>
+        <v>139.66</v>
       </c>
       <c r="J38" s="23">
         <f>H38*$N$34</f>
-        <v>1458.3609472000001</v>
+        <v>2932.7357632000003</v>
       </c>
       <c r="K38" s="36"/>
       <c r="L38" s="23"/>
@@ -2270,12 +2600,12 @@
       </c>
       <c r="E41" s="22">
         <f>E34+D34</f>
-        <v>110000</v>
+        <v>210000</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22">
         <f>E41*30</f>
-        <v>3300000</v>
+        <v>6300000</v>
       </c>
       <c r="H41" s="5">
         <f>IF(E41 &lt;(24*60*60)*1000,24,E41/60/60/1000)*$Q$40</f>
@@ -2283,7 +2613,7 @@
       </c>
       <c r="I41" s="24">
         <f>G41/100000*$N$40*($Q$13/$N$42)</f>
-        <v>1.8480000000000001</v>
+        <v>3.528</v>
       </c>
       <c r="J41" s="24">
         <f>H41*$N$41*30</f>
@@ -2311,12 +2641,12 @@
       </c>
       <c r="E42" s="22">
         <f>E35+D35</f>
-        <v>1100000</v>
+        <v>2100000</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="22">
         <f>E42*30</f>
-        <v>33000000</v>
+        <v>63000000</v>
       </c>
       <c r="H42" s="5">
         <f>IF(E42 &lt;(24*60*60)*1000,24,E42/60/60/1000)*$Q$40</f>
@@ -2324,7 +2654,7 @@
       </c>
       <c r="I42" s="24">
         <f>G42/100000*$N$40*($Q$13/$N$42)</f>
-        <v>18.48</v>
+        <v>35.28</v>
       </c>
       <c r="J42" s="24">
         <f>H42*$N$41*30</f>
@@ -2352,12 +2682,12 @@
       </c>
       <c r="E43" s="22">
         <f>E36+D36</f>
-        <v>11000000</v>
+        <v>21000000</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="22">
         <f>E43*30</f>
-        <v>330000000</v>
+        <v>630000000</v>
       </c>
       <c r="H43" s="5">
         <f>IF(E43 &lt;(24*60*60)*1000,24,E43/60/60/1000)*$Q$40</f>
@@ -2365,7 +2695,7 @@
       </c>
       <c r="I43" s="24">
         <f>G43/100000*$N$40*($Q$13/$N$42)</f>
-        <v>184.8</v>
+        <v>352.8</v>
       </c>
       <c r="J43" s="24">
         <f>H43*$N$41*30</f>
@@ -2391,7 +2721,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="23">
         <f>SUM(I41:I43)</f>
-        <v>205.12800000000001</v>
+        <v>391.608</v>
       </c>
       <c r="J44" s="23">
         <f>SUM(J41:J43)</f>
@@ -2426,7 +2756,7 @@
       <c r="G46" s="18"/>
       <c r="H46" s="29">
         <f>I38+J38+H31+H25+I44+J44</f>
-        <v>2421.1303472</v>
+        <v>4148.5851632000004</v>
       </c>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
@@ -2447,4 +2777,2013 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="5"/>
+    <col min="4" max="4" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="5"/>
+    <col min="10" max="10" width="15.33203125" style="5" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" style="5" customWidth="1"/>
+    <col min="13" max="14" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="5" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18">
+      <c r="M2" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" s="53"/>
+    </row>
+    <row r="3" spans="2:18" s="8" customFormat="1">
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="4"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="M5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="49"/>
+      <c r="O5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="47">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8">
+        <f>E6</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="39">
+        <f>VLOOKUP(D6,$M$30:$N$57,2,FALSE)</f>
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="H6" s="9">
+        <f>30*24*G6*F6</f>
+        <v>58.32</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="M6" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="56"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="32"/>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="47">
+        <v>42</v>
+      </c>
+      <c r="F7" s="8">
+        <f>E7</f>
+        <v>42</v>
+      </c>
+      <c r="G7" s="39">
+        <f>VLOOKUP(D7,$M$30:$N$57,2,FALSE)</f>
+        <v>0.42</v>
+      </c>
+      <c r="H7" s="9">
+        <f>30*24*G7*F7</f>
+        <v>12700.8</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="M7" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="56"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="32"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="47">
+        <v>62</v>
+      </c>
+      <c r="F8" s="8">
+        <f>E8</f>
+        <v>62</v>
+      </c>
+      <c r="G8" s="39">
+        <f>VLOOKUP(D8,$M$30:$N$57,2,FALSE)</f>
+        <v>1.68</v>
+      </c>
+      <c r="H8" s="9">
+        <f>30*24*G8*F8</f>
+        <v>74995.199999999997</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="32"/>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="47">
+        <v>31</v>
+      </c>
+      <c r="F9" s="8">
+        <f>E9</f>
+        <v>31</v>
+      </c>
+      <c r="G9" s="39">
+        <f>VLOOKUP(D9,$M$30:$N$57,2,FALSE)</f>
+        <v>0.105</v>
+      </c>
+      <c r="H9" s="9">
+        <f>30*24*G9*F9</f>
+        <v>2343.6</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="32"/>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="47">
+        <v>43</v>
+      </c>
+      <c r="F10" s="8">
+        <f>E10</f>
+        <v>43</v>
+      </c>
+      <c r="G10" s="39">
+        <f>VLOOKUP(D10,$M$30:$N$57,2,FALSE)</f>
+        <v>0.21</v>
+      </c>
+      <c r="H10" s="9">
+        <f>30*24*G10*F10</f>
+        <v>6501.5999999999995</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="32"/>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="47">
+        <v>4</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" ref="F11:F26" si="0">E11</f>
+        <v>4</v>
+      </c>
+      <c r="G11" s="39">
+        <f>VLOOKUP(D11,$M$30:$N$57,2,FALSE)</f>
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" ref="H11:H16" si="1">30*24*G11*F11</f>
+        <v>2413.44</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="32"/>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="47">
+        <v>2</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G12" s="39">
+        <f t="shared" ref="G12:G23" si="2">VLOOKUP(D12,$M$30:$N$57,2,FALSE)</f>
+        <v>0.24440000000000001</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" ref="H12:H23" si="3">30*24*G12*F12</f>
+        <v>351.93600000000004</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="32"/>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="47">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G13" s="39">
+        <f t="shared" si="2"/>
+        <v>0.25769999999999998</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="3"/>
+        <v>2040.9839999999999</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="32"/>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="47">
+        <v>2</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G14" s="39">
+        <f t="shared" si="2"/>
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" si="3"/>
+        <v>24.335999999999999</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="32"/>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="47">
+        <v>11</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G15" s="39">
+        <f t="shared" si="2"/>
+        <v>1.111E-2</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="3"/>
+        <v>87.991200000000006</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="32"/>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="47">
+        <v>28</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="G16" s="39">
+        <f t="shared" si="2"/>
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="3"/>
+        <v>143.136</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="32"/>
+    </row>
+    <row r="17" spans="2:18">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="47">
+        <v>15</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G17" s="39">
+        <f t="shared" si="2"/>
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" si="3"/>
+        <v>449.28</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="32"/>
+    </row>
+    <row r="18" spans="2:18">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="47">
+        <v>5</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G18" s="39">
+        <f t="shared" si="2"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" si="3"/>
+        <v>277.2</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="32"/>
+    </row>
+    <row r="19" spans="2:18">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="47">
+        <v>76</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="G19" s="39">
+        <f t="shared" si="2"/>
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="H19" s="9">
+        <f t="shared" si="3"/>
+        <v>29111.040000000001</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="32"/>
+    </row>
+    <row r="20" spans="2:18">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="47">
+        <v>94</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="G20" s="39">
+        <f t="shared" si="2"/>
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="H20" s="9">
+        <f t="shared" si="3"/>
+        <v>9001.44</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="32"/>
+    </row>
+    <row r="21" spans="2:18">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="47">
+        <v>200</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="G21" s="39">
+        <f t="shared" si="2"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H21" s="9">
+        <f t="shared" si="3"/>
+        <v>9648</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="32"/>
+    </row>
+    <row r="22" spans="2:18">
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="47">
+        <v>158</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="G22" s="39">
+        <f t="shared" ref="G22:G24" si="4">VLOOKUP(D22,$M$30:$N$57,2,FALSE)</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="H22" s="9">
+        <f t="shared" ref="H22:H24" si="5">30*24*G22*F22</f>
+        <v>30260.16</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="32"/>
+    </row>
+    <row r="23" spans="2:18">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="47">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G23" s="39">
+        <f t="shared" si="4"/>
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" si="5"/>
+        <v>4.68</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="32"/>
+    </row>
+    <row r="24" spans="2:18">
+      <c r="B24" s="4"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="6"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="6"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="6"/>
+    </row>
+    <row r="25" spans="2:18">
+      <c r="B25" s="4"/>
+      <c r="D25" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="42">
+        <v>388</v>
+      </c>
+      <c r="F25" s="28">
+        <f t="shared" si="0"/>
+        <v>388</v>
+      </c>
+      <c r="G25" s="39"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="6"/>
+      <c r="M25" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="N25" s="50"/>
+      <c r="O25" s="6"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="6"/>
+    </row>
+    <row r="26" spans="2:18">
+      <c r="B26" s="4"/>
+      <c r="D26" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="42">
+        <v>290</v>
+      </c>
+      <c r="F26" s="28">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="G26" s="39"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N26" s="42">
+        <v>8.8739999999999999E-2</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="6"/>
+    </row>
+    <row r="27" spans="2:18">
+      <c r="B27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="12">
+        <f>SUM(H6:H26)</f>
+        <v>180413.14319999999</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="6"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="6"/>
+    </row>
+    <row r="28" spans="2:18">
+      <c r="B28" s="4"/>
+      <c r="I28" s="6"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="6"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="6"/>
+    </row>
+    <row r="29" spans="2:18">
+      <c r="B29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="6"/>
+      <c r="M29" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="N29" s="42"/>
+      <c r="O29" s="6"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="6"/>
+    </row>
+    <row r="30" spans="2:18">
+      <c r="B30" s="4"/>
+      <c r="C30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13">
+        <f>D30*$Q$32</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="14">
+        <f>D30/24/60/60*($Q$30)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="13">
+        <f>(E30+D30)*30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="9">
+        <f>D30*($Q$31/1000)*$N$26</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="6"/>
+      <c r="M30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N30" s="43">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q30" s="42">
+        <v>40</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18">
+      <c r="B31" s="4"/>
+      <c r="C31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="13">
+        <f>24*4*(36+5+9+3+5+11+6)</f>
+        <v>7200</v>
+      </c>
+      <c r="E31" s="13">
+        <f>68900000/14</f>
+        <v>4921428.5714285718</v>
+      </c>
+      <c r="F31" s="14">
+        <f>D31/24/60/60*($Q$30)</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="G31" s="13">
+        <f>(E31+D31)*30</f>
+        <v>147858857.14285716</v>
+      </c>
+      <c r="H31" s="9">
+        <f>D31*($Q$31/1000)*$N$26</f>
+        <v>0.63892800000000005</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="M31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N31" s="43">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q31" s="42">
+        <v>1</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18">
+      <c r="B32" s="4"/>
+      <c r="C32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="13">
+        <f>24*4*(253+2296+27+72+49+447+0+1938+315) +24*4*(950+3513)</f>
+        <v>946560</v>
+      </c>
+      <c r="E32" s="13">
+        <f>1300000000/14</f>
+        <v>92857142.857142851</v>
+      </c>
+      <c r="F32" s="14">
+        <f>D32/24/60/60*($Q$30)</f>
+        <v>438.22222222222223</v>
+      </c>
+      <c r="G32" s="13">
+        <f>(E32+D32)*30</f>
+        <v>2814111085.7142854</v>
+      </c>
+      <c r="H32" s="9">
+        <f>D32*($Q$31/1000)*$N$26</f>
+        <v>83.997734399999999</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="M32" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N32" s="43">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="6"/>
+    </row>
+    <row r="33" spans="2:18">
+      <c r="B33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="16">
+        <f>SUM(H30:H32)</f>
+        <v>84.636662400000006</v>
+      </c>
+      <c r="I33" s="6"/>
+      <c r="M33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="N33" s="43">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="6"/>
+    </row>
+    <row r="34" spans="2:18">
+      <c r="B34" s="4"/>
+      <c r="I34" s="6"/>
+      <c r="M34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N34" s="43">
+        <v>1.111E-2</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="6"/>
+    </row>
+    <row r="35" spans="2:18" s="8" customFormat="1">
+      <c r="B35" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="19">
+        <f>H33+H27</f>
+        <v>180497.7798624</v>
+      </c>
+      <c r="I35" s="20"/>
+      <c r="M35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N35" s="43">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="32"/>
+    </row>
+    <row r="36" spans="2:18" s="8" customFormat="1">
+      <c r="H36" s="23"/>
+      <c r="M36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="N36" s="43">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="32"/>
+    </row>
+    <row r="37" spans="2:18" s="8" customFormat="1">
+      <c r="H37" s="23"/>
+      <c r="M37" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="N37" s="43">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q37" s="47"/>
+      <c r="R37" s="32"/>
+    </row>
+    <row r="38" spans="2:18" s="8" customFormat="1">
+      <c r="H38" s="23"/>
+      <c r="M38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N38" s="43">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q38" s="47"/>
+      <c r="R38" s="32"/>
+    </row>
+    <row r="39" spans="2:18" s="8" customFormat="1">
+      <c r="H39" s="23"/>
+      <c r="M39" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="N39" s="43">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q39" s="47"/>
+      <c r="R39" s="32"/>
+    </row>
+    <row r="40" spans="2:18" s="8" customFormat="1">
+      <c r="H40" s="23"/>
+      <c r="M40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N40" s="43">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q40" s="47"/>
+      <c r="R40" s="32"/>
+    </row>
+    <row r="41" spans="2:18" s="8" customFormat="1">
+      <c r="H41" s="23"/>
+      <c r="M41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" s="43">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="O41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q41" s="47"/>
+      <c r="R41" s="32"/>
+    </row>
+    <row r="42" spans="2:18" s="8" customFormat="1">
+      <c r="H42" s="23"/>
+      <c r="M42" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N42" s="43">
+        <v>0.104</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="32"/>
+    </row>
+    <row r="43" spans="2:18" s="8" customFormat="1">
+      <c r="H43" s="23"/>
+      <c r="M43" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="N43" s="44">
+        <v>0.105</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="32"/>
+    </row>
+    <row r="44" spans="2:18" s="8" customFormat="1">
+      <c r="H44" s="23"/>
+      <c r="M44" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N44" s="43">
+        <v>0.12</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q44" s="47"/>
+      <c r="R44" s="32"/>
+    </row>
+    <row r="45" spans="2:18">
+      <c r="M45" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N45" s="43">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q45" s="42"/>
+      <c r="R45" s="6"/>
+    </row>
+    <row r="46" spans="2:18" s="8" customFormat="1">
+      <c r="B46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="3"/>
+      <c r="M46" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="N46" s="44">
+        <v>0.21</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q46" s="47"/>
+      <c r="R46" s="32"/>
+    </row>
+    <row r="47" spans="2:18">
+      <c r="B47" s="4"/>
+      <c r="K47" s="6"/>
+      <c r="M47" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N47" s="43">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q47" s="42"/>
+      <c r="R47" s="6"/>
+    </row>
+    <row r="48" spans="2:18">
+      <c r="B48" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="6"/>
+      <c r="M48" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N48" s="43">
+        <v>0.24440000000000001</v>
+      </c>
+      <c r="O48" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q48" s="42"/>
+      <c r="R48" s="6"/>
+    </row>
+    <row r="49" spans="2:18">
+      <c r="B49" s="4"/>
+      <c r="D49" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="41">
+        <v>30</v>
+      </c>
+      <c r="F49" s="21"/>
+      <c r="G49" s="39">
+        <f>VLOOKUP(D49,$M$30:$N$57,2,FALSE)</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H49" s="9">
+        <f>30*24*G49*E49</f>
+        <v>1447.2</v>
+      </c>
+      <c r="K49" s="6"/>
+      <c r="M49" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="N49" s="43">
+        <v>0.25769999999999998</v>
+      </c>
+      <c r="O49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q49" s="42"/>
+      <c r="R49" s="6"/>
+    </row>
+    <row r="50" spans="2:18">
+      <c r="B50" s="4"/>
+      <c r="D50" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="41">
+        <v>30</v>
+      </c>
+      <c r="F50" s="21"/>
+      <c r="G50" s="39">
+        <f>VLOOKUP(D50,$M$30:$N$57,2,FALSE)</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="H50" s="9">
+        <f>30*24*G50*E50</f>
+        <v>5745.6</v>
+      </c>
+      <c r="K50" s="6"/>
+      <c r="M50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N50" s="43">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q50" s="42"/>
+      <c r="R50" s="6"/>
+    </row>
+    <row r="51" spans="2:18">
+      <c r="B51" s="4"/>
+      <c r="D51" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="41">
+        <v>11</v>
+      </c>
+      <c r="F51" s="21"/>
+      <c r="G51" s="39">
+        <f>VLOOKUP(D51,$M$30:$N$57,2,FALSE)</f>
+        <v>0.25769999999999998</v>
+      </c>
+      <c r="H51" s="9">
+        <f>30*24*G51*E51</f>
+        <v>2040.9839999999999</v>
+      </c>
+      <c r="K51" s="6"/>
+      <c r="M51" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="N51" s="44">
+        <v>0.42</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q51" s="42"/>
+      <c r="R51" s="6"/>
+    </row>
+    <row r="52" spans="2:18">
+      <c r="B52" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="12">
+        <f>SUM(H49:H51)</f>
+        <v>9233.7839999999997</v>
+      </c>
+      <c r="K52" s="6"/>
+      <c r="M52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N52" s="43">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q52" s="42"/>
+      <c r="R52" s="6"/>
+    </row>
+    <row r="53" spans="2:18">
+      <c r="B53" s="4"/>
+      <c r="K53" s="6"/>
+      <c r="M53" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N53" s="43">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q53" s="42"/>
+      <c r="R53" s="6"/>
+    </row>
+    <row r="54" spans="2:18">
+      <c r="B54" s="7" t="str">
+        <f>B29</f>
+        <v>Traffic</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8" t="str">
+        <f>D29</f>
+        <v>hits/day</v>
+      </c>
+      <c r="E54" s="8" t="str">
+        <f>E29</f>
+        <v>mid tier/day</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8" t="str">
+        <f>G29</f>
+        <v>calls/month</v>
+      </c>
+      <c r="H54" s="8" t="str">
+        <f>H29</f>
+        <v>$monthly (edge)</v>
+      </c>
+      <c r="I54" s="8"/>
+      <c r="K54" s="6"/>
+      <c r="M54" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="N54" s="44">
+        <v>0.84</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P54" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q54" s="42">
+        <v>9</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18">
+      <c r="B55" s="4"/>
+      <c r="C55" s="5" t="str">
+        <f>C30</f>
+        <v>dev</v>
+      </c>
+      <c r="D55" s="13">
+        <f>D30</f>
+        <v>0</v>
+      </c>
+      <c r="E55" s="13">
+        <f>E30*$Q$54</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13">
+        <f>(E55+D55)*30</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="9">
+        <f>D55*($Q$31/1000)*$N$26</f>
+        <v>0</v>
+      </c>
+      <c r="K55" s="6"/>
+      <c r="M55" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N55" s="43">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q55" s="42"/>
+      <c r="R55" s="6"/>
+    </row>
+    <row r="56" spans="2:18">
+      <c r="B56" s="4"/>
+      <c r="C56" s="5" t="str">
+        <f>C31</f>
+        <v>test</v>
+      </c>
+      <c r="D56" s="13">
+        <f>D31</f>
+        <v>7200</v>
+      </c>
+      <c r="E56" s="13">
+        <f>E31*$Q$54</f>
+        <v>44292857.142857149</v>
+      </c>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13">
+        <f>(E56+D56)*30</f>
+        <v>1329001714.2857144</v>
+      </c>
+      <c r="H56" s="9">
+        <f>D56*($Q$31/1000)*$N$26</f>
+        <v>0.63892800000000005</v>
+      </c>
+      <c r="K56" s="6"/>
+      <c r="M56" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="N56" s="44">
+        <v>1.68</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q56" s="42"/>
+      <c r="R56" s="6"/>
+    </row>
+    <row r="57" spans="2:18">
+      <c r="B57" s="4"/>
+      <c r="C57" s="5" t="str">
+        <f>C32</f>
+        <v>prod</v>
+      </c>
+      <c r="D57" s="13">
+        <f>D32</f>
+        <v>946560</v>
+      </c>
+      <c r="E57" s="13">
+        <f>E32*$Q$54</f>
+        <v>835714285.71428561</v>
+      </c>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13">
+        <f>(E57+D57)*30</f>
+        <v>25099825371.42857</v>
+      </c>
+      <c r="H57" s="9">
+        <f>D57*($Q$31/1000)*$N$26</f>
+        <v>83.997734399999999</v>
+      </c>
+      <c r="K57" s="6"/>
+      <c r="M57" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N57" s="43">
+        <v>2.3940000000000001</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q57" s="42"/>
+      <c r="R57" s="6"/>
+    </row>
+    <row r="58" spans="2:18">
+      <c r="B58" s="7" t="str">
+        <f>B33</f>
+        <v>Subtotal Traffic</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="23">
+        <f>H33</f>
+        <v>84.636662400000006</v>
+      </c>
+      <c r="K58" s="6"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="42"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q58" s="42">
+        <v>100</v>
+      </c>
+      <c r="R58" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18">
+      <c r="B59" s="4"/>
+      <c r="K59" s="6"/>
+      <c r="M59" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N59" s="42"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q59" s="42">
+        <v>512</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18">
+      <c r="B60" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K60" s="32"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N60" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18">
+      <c r="B61" s="4"/>
+      <c r="C61" s="5" t="str">
+        <f>C55</f>
+        <v>dev</v>
+      </c>
+      <c r="D61" s="13">
+        <f t="shared" ref="D61" si="6">D55</f>
+        <v>0</v>
+      </c>
+      <c r="E61" s="13">
+        <f>E55</f>
+        <v>0</v>
+      </c>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13">
+        <f>30*(E61+D61)</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="13">
+        <f>((D61+(E61*(1-$Q$61-$Q$65)))*30*($Q$59/1000)*($Q$58/1000))+           ((E61*$Q$61)*30*($Q$62/1000)*($Q$63/1000))+           ((E61*$Q$65)*30*($Q$66/1000)*($Q$67/1000))</f>
+        <v>0</v>
+      </c>
+      <c r="I61" s="9">
+        <f>(G61/1000000)*$N$60</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="24">
+        <f>H61*$N$61</f>
+        <v>0</v>
+      </c>
+      <c r="K61" s="35"/>
+      <c r="L61" s="24"/>
+      <c r="M61" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N61" s="42">
+        <v>1.6670000000000001E-5</v>
+      </c>
+      <c r="O61" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P61" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q61" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="R61" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18">
+      <c r="B62" s="4"/>
+      <c r="C62" s="5" t="str">
+        <f t="shared" ref="C62:D63" si="7">C56</f>
+        <v>test</v>
+      </c>
+      <c r="D62" s="13">
+        <f t="shared" si="7"/>
+        <v>7200</v>
+      </c>
+      <c r="E62" s="13">
+        <f>E56</f>
+        <v>44292857.142857149</v>
+      </c>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13">
+        <f>30*(E62+D62)</f>
+        <v>1329001714.2857144</v>
+      </c>
+      <c r="H62" s="13">
+        <f>((D62+(E62*(1-$Q$61-$Q$65)))*30*($Q$59/1000)*($Q$58/1000))+           ((E62*$Q$61)*30*($Q$62/1000)*($Q$63/1000))+           ((E62*$Q$65)*30*($Q$66/1000)*($Q$67/1000))</f>
+        <v>442162911.0857144</v>
+      </c>
+      <c r="I62" s="9">
+        <f>(G62/1000000)*$N$60</f>
+        <v>265.80034285714288</v>
+      </c>
+      <c r="J62" s="24">
+        <f>H62*$N$61</f>
+        <v>7370.8557277988593</v>
+      </c>
+      <c r="K62" s="35"/>
+      <c r="L62" s="24"/>
+      <c r="M62" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="N62" s="46">
+        <v>1000000</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="P62" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q62" s="46">
+        <v>1000</v>
+      </c>
+      <c r="R62" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18">
+      <c r="B63" s="4"/>
+      <c r="C63" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>prod</v>
+      </c>
+      <c r="D63" s="13">
+        <f t="shared" si="7"/>
+        <v>946560</v>
+      </c>
+      <c r="E63" s="13">
+        <f>E57</f>
+        <v>835714285.71428561</v>
+      </c>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13">
+        <f>30*(E63+D63)</f>
+        <v>25099825371.42857</v>
+      </c>
+      <c r="H63" s="13">
+        <f>((D63+(E63*(1-$Q$61-$Q$65)))*30*($Q$59/1000)*($Q$58/1000))+           ((E63*$Q$61)*30*($Q$62/1000)*($Q$63/1000))+           ((E63*$Q$65)*30*($Q$66/1000)*($Q$67/1000))</f>
+        <v>8343941687.5885715</v>
+      </c>
+      <c r="I63" s="9">
+        <f>(G63/1000000)*$N$60</f>
+        <v>5019.9650742857148</v>
+      </c>
+      <c r="J63" s="24">
+        <f>H63*$N$61</f>
+        <v>139093.50793210149</v>
+      </c>
+      <c r="K63" s="35"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N63" s="46">
+        <v>1600000</v>
+      </c>
+      <c r="O63" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P63" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q63" s="42">
+        <v>1024</v>
+      </c>
+      <c r="R63" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18">
+      <c r="B64" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13">
+        <f>SUM(G61:G63)</f>
+        <v>26428827085.714283</v>
+      </c>
+      <c r="H64" s="13">
+        <f>SUM(H61:H63)</f>
+        <v>8786104598.6742859</v>
+      </c>
+      <c r="I64" s="9">
+        <f>(G64/1000000)*$N$60</f>
+        <v>5285.7654171428567</v>
+      </c>
+      <c r="J64" s="24">
+        <f>H64*$N$61</f>
+        <v>146464.36365990035</v>
+      </c>
+      <c r="K64" s="35"/>
+      <c r="L64" s="24"/>
+      <c r="M64" s="26"/>
+      <c r="N64" s="46"/>
+      <c r="O64" s="6"/>
+      <c r="Q64" s="42"/>
+      <c r="R64" s="6"/>
+    </row>
+    <row r="65" spans="2:18">
+      <c r="B65" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27">
+        <f>IF(G64&gt;N62,G64-N62,0)</f>
+        <v>26427827085.714283</v>
+      </c>
+      <c r="H65" s="27">
+        <f>IF(H64&gt;N63,H64-N63,0)</f>
+        <v>8784504598.6742859</v>
+      </c>
+      <c r="I65" s="12">
+        <f>(G65/1000000)*$N$60</f>
+        <v>5285.5654171428569</v>
+      </c>
+      <c r="J65" s="23">
+        <f>H65*$N$61</f>
+        <v>146437.69165990036</v>
+      </c>
+      <c r="K65" s="36"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="42"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65" s="42">
+        <v>1E-3</v>
+      </c>
+      <c r="R65" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18">
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="42"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q66" s="46">
+        <f>3*60*1000</f>
+        <v>180000</v>
+      </c>
+      <c r="R66" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18">
+      <c r="B67" s="4"/>
+      <c r="K67" s="6"/>
+      <c r="M67" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="N67" s="42"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q67" s="42">
+        <v>1024</v>
+      </c>
+      <c r="R67" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18">
+      <c r="B68" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H68" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I68" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J68" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="K68" s="37"/>
+      <c r="L68" s="28"/>
+      <c r="M68" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="N68" s="42">
+        <v>1.4E-2</v>
+      </c>
+      <c r="O68" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q68" s="42"/>
+      <c r="R68" s="6"/>
+    </row>
+    <row r="69" spans="2:18">
+      <c r="B69" s="4"/>
+      <c r="C69" s="5" t="str">
+        <f>C61</f>
+        <v>dev</v>
+      </c>
+      <c r="E69" s="22">
+        <f>E61+D61</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22">
+        <f>E69*30</f>
+        <v>0</v>
+      </c>
+      <c r="H69" s="5">
+        <f>IF(E69 &gt; 0,IF(E69 &lt;(24*60*60)*1000,24,E69/60/60/1000)*$Q$69,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I69" s="24">
+        <f>G69/100000*$N$68*($Q$31/$N$70)</f>
+        <v>0</v>
+      </c>
+      <c r="J69" s="24">
+        <f>H69*$N$69*30</f>
+        <v>0</v>
+      </c>
+      <c r="K69" s="35"/>
+      <c r="L69" s="24"/>
+      <c r="M69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N69" s="42">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O69" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q69" s="42">
+        <v>30</v>
+      </c>
+      <c r="R69" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18">
+      <c r="B70" s="4"/>
+      <c r="C70" s="5" t="str">
+        <f t="shared" ref="C70:C71" si="8">C62</f>
+        <v>test</v>
+      </c>
+      <c r="E70" s="22">
+        <f>E62+D62</f>
+        <v>44300057.142857149</v>
+      </c>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22">
+        <f>E70*30</f>
+        <v>1329001714.2857144</v>
+      </c>
+      <c r="H70" s="5">
+        <f>IF(E70 &gt; 0,IF(E70 &lt;(24*60*60)*1000,24,E70/60/60/1000)*$Q$69,0)</f>
+        <v>720</v>
+      </c>
+      <c r="I70" s="24">
+        <f>G70/100000*$N$68*($Q$31/$N$70)</f>
+        <v>744.24095999999997</v>
+      </c>
+      <c r="J70" s="24">
+        <f>H70*$N$69*30</f>
+        <v>323.99999999999994</v>
+      </c>
+      <c r="K70" s="35"/>
+      <c r="L70" s="24"/>
+      <c r="M70" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N70" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="O70" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q70" s="48"/>
+      <c r="R70" s="6"/>
+    </row>
+    <row r="71" spans="2:18">
+      <c r="B71" s="4"/>
+      <c r="C71" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>prod</v>
+      </c>
+      <c r="E71" s="22">
+        <f>E63+D63</f>
+        <v>836660845.71428561</v>
+      </c>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22">
+        <f>E71*30</f>
+        <v>25099825371.42857</v>
+      </c>
+      <c r="H71" s="57">
+        <f>IF(E71 &gt; 0,IF(E71 &lt;(24*60*60)*1000,24,E71/60/60/1000)*$Q$69,0)</f>
+        <v>6972.1737142857137</v>
+      </c>
+      <c r="I71" s="24">
+        <f>G71/100000*$N$68*($Q$31/$N$70)</f>
+        <v>14055.902208</v>
+      </c>
+      <c r="J71" s="24">
+        <f>H71*$N$69*30</f>
+        <v>3137.4781714285709</v>
+      </c>
+      <c r="K71" s="35"/>
+      <c r="L71" s="24"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="50"/>
+      <c r="O71" s="6"/>
+      <c r="Q71" s="50"/>
+      <c r="R71" s="6"/>
+    </row>
+    <row r="72" spans="2:18">
+      <c r="B72" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="23">
+        <f>SUM(I69:I71)</f>
+        <v>14800.143167999999</v>
+      </c>
+      <c r="J72" s="23">
+        <f>SUM(J69:J71)</f>
+        <v>3461.4781714285709</v>
+      </c>
+      <c r="K72" s="36"/>
+      <c r="L72" s="23"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="50"/>
+      <c r="O72" s="6"/>
+      <c r="Q72" s="50"/>
+      <c r="R72" s="6"/>
+    </row>
+    <row r="73" spans="2:18">
+      <c r="B73" s="4"/>
+      <c r="K73" s="6"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="51"/>
+      <c r="O73" s="11"/>
+      <c r="P73" s="10"/>
+      <c r="Q73" s="51"/>
+      <c r="R73" s="11"/>
+    </row>
+    <row r="74" spans="2:18" s="8" customFormat="1">
+      <c r="B74" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="29">
+        <f>I65+J65+H58+H52+I72+J72</f>
+        <v>179303.29907887179</v>
+      </c>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="20"/>
+    </row>
+    <row r="77" spans="2:18" s="8" customFormat="1">
+      <c r="B77" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="D7:E23">
+    <sortCondition ref="D6"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add in aws api gateway pricing to complex model
</commit_message>
<xml_diff>
--- a/api-lambda-mock/ec2-vs-lambda.xlsx
+++ b/api-lambda-mock/ec2-vs-lambda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13600" yWindow="7780" windowWidth="35480" windowHeight="30920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="19660" yWindow="1500" windowWidth="29720" windowHeight="31420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple EC2-vs-Lambda" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="132">
   <si>
     <t>AWS EC2 costs for a small SOA architecture</t>
   </si>
@@ -498,6 +498,36 @@
   </si>
   <si>
     <t>mid medium/light</t>
+  </si>
+  <si>
+    <t>API GATEWAY</t>
+  </si>
+  <si>
+    <t>per mill calls</t>
+  </si>
+  <si>
+    <t>$/GB out</t>
+  </si>
+  <si>
+    <t>Data Transfer</t>
+  </si>
+  <si>
+    <t>Subtotals API Gateway</t>
+  </si>
+  <si>
+    <t>$ for calls</t>
+  </si>
+  <si>
+    <t>$ for xfer out</t>
+  </si>
+  <si>
+    <t>per day</t>
+  </si>
+  <si>
+    <t>per month</t>
+  </si>
+  <si>
+    <t>AWS API Gateway (edge)</t>
   </si>
 </sst>
 </file>
@@ -710,7 +740,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -833,8 +863,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -923,8 +967,13 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="122">
+  <cellStyles count="136">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -986,6 +1035,13 @@
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1046,6 +1102,13 @@
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2781,10 +2844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R77"/>
+  <dimension ref="B2:R82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q67" sqref="Q67"/>
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2881,7 +2944,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="39">
-        <f>VLOOKUP(D6,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" ref="G6:G11" si="0">VLOOKUP(D6,$M$30:$N$57,2,FALSE)</f>
         <v>1.6199999999999999E-2</v>
       </c>
       <c r="H6" s="9">
@@ -2912,7 +2975,7 @@
         <v>42</v>
       </c>
       <c r="G7" s="39">
-        <f>VLOOKUP(D7,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
       <c r="H7" s="9">
@@ -2943,7 +3006,7 @@
         <v>62</v>
       </c>
       <c r="G8" s="39">
-        <f>VLOOKUP(D8,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1.68</v>
       </c>
       <c r="H8" s="9">
@@ -2972,7 +3035,7 @@
         <v>31</v>
       </c>
       <c r="G9" s="39">
-        <f>VLOOKUP(D9,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.105</v>
       </c>
       <c r="H9" s="9">
@@ -3001,7 +3064,7 @@
         <v>43</v>
       </c>
       <c r="G10" s="39">
-        <f>VLOOKUP(D10,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
       <c r="H10" s="9">
@@ -3026,15 +3089,15 @@
         <v>4</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" ref="F11:F26" si="0">E11</f>
+        <f t="shared" ref="F11:F26" si="1">E11</f>
         <v>4</v>
       </c>
       <c r="G11" s="39">
-        <f>VLOOKUP(D11,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.83799999999999997</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" ref="H11:H16" si="1">30*24*G11*F11</f>
+        <f t="shared" ref="H11" si="2">30*24*G11*F11</f>
         <v>2413.44</v>
       </c>
       <c r="I11" s="6"/>
@@ -3055,15 +3118,15 @@
         <v>2</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G12" s="39">
-        <f t="shared" ref="G12:G23" si="2">VLOOKUP(D12,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" ref="G12:G21" si="3">VLOOKUP(D12,$M$30:$N$57,2,FALSE)</f>
         <v>0.24440000000000001</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" ref="H12:H23" si="3">30*24*G12*F12</f>
+        <f t="shared" ref="H12:H21" si="4">30*24*G12*F12</f>
         <v>351.93600000000004</v>
       </c>
       <c r="I12" s="6"/>
@@ -3084,15 +3147,15 @@
         <v>11</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G13" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25769999999999998</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2040.9839999999999</v>
       </c>
       <c r="I13" s="6"/>
@@ -3113,15 +3176,15 @@
         <v>2</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G14" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6899999999999998E-2</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24.335999999999999</v>
       </c>
       <c r="I14" s="6"/>
@@ -3142,15 +3205,15 @@
         <v>11</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G15" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.111E-2</v>
       </c>
       <c r="H15" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87.991200000000006</v>
       </c>
       <c r="I15" s="6"/>
@@ -3171,15 +3234,15 @@
         <v>28</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="G16" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>143.136</v>
       </c>
       <c r="I16" s="6"/>
@@ -3200,15 +3263,15 @@
         <v>15</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G17" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.1599999999999998E-2</v>
       </c>
       <c r="H17" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>449.28</v>
       </c>
       <c r="I17" s="6"/>
@@ -3229,15 +3292,15 @@
         <v>5</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G18" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>277.2</v>
       </c>
       <c r="I18" s="6"/>
@@ -3258,15 +3321,15 @@
         <v>76</v>
       </c>
       <c r="F19" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="G19" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.53200000000000003</v>
       </c>
       <c r="H19" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29111.040000000001</v>
       </c>
       <c r="I19" s="6"/>
@@ -3287,15 +3350,15 @@
         <v>94</v>
       </c>
       <c r="F20" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
       <c r="G20" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13300000000000001</v>
       </c>
       <c r="H20" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9001.44</v>
       </c>
       <c r="I20" s="6"/>
@@ -3316,15 +3379,15 @@
         <v>200</v>
       </c>
       <c r="F21" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="G21" s="39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="H21" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9648</v>
       </c>
       <c r="I21" s="6"/>
@@ -3345,15 +3408,15 @@
         <v>158</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>158</v>
       </c>
       <c r="G22" s="39">
-        <f t="shared" ref="G22:G24" si="4">VLOOKUP(D22,$M$30:$N$57,2,FALSE)</f>
+        <f t="shared" ref="G22:G23" si="5">VLOOKUP(D22,$M$30:$N$57,2,FALSE)</f>
         <v>0.26600000000000001</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" ref="H22:H24" si="5">30*24*G22*F22</f>
+        <f t="shared" ref="H22:H23" si="6">30*24*G22*F22</f>
         <v>30260.16</v>
       </c>
       <c r="I22" s="6"/>
@@ -3374,15 +3437,15 @@
         <v>1</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G23" s="39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.4999999999999997E-3</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.68</v>
       </c>
       <c r="I23" s="6"/>
@@ -3416,7 +3479,7 @@
         <v>388</v>
       </c>
       <c r="F25" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>388</v>
       </c>
       <c r="G25" s="39"/>
@@ -3439,7 +3502,7 @@
         <v>290</v>
       </c>
       <c r="F26" s="28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>290</v>
       </c>
       <c r="G26" s="39"/>
@@ -4098,11 +4161,11 @@
     <row r="55" spans="2:18">
       <c r="B55" s="4"/>
       <c r="C55" s="5" t="str">
-        <f>C30</f>
+        <f t="shared" ref="C55:D57" si="7">C30</f>
         <v>dev</v>
       </c>
       <c r="D55" s="13">
-        <f>D30</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E55" s="13">
@@ -4134,11 +4197,11 @@
     <row r="56" spans="2:18">
       <c r="B56" s="4"/>
       <c r="C56" s="5" t="str">
-        <f>C31</f>
+        <f t="shared" si="7"/>
         <v>test</v>
       </c>
       <c r="D56" s="13">
-        <f>D31</f>
+        <f t="shared" si="7"/>
         <v>7200</v>
       </c>
       <c r="E56" s="13">
@@ -4170,11 +4233,11 @@
     <row r="57" spans="2:18">
       <c r="B57" s="4"/>
       <c r="C57" s="5" t="str">
-        <f>C32</f>
+        <f t="shared" si="7"/>
         <v>prod</v>
       </c>
       <c r="D57" s="13">
-        <f>D32</f>
+        <f t="shared" si="7"/>
         <v>946560</v>
       </c>
       <c r="E57" s="13">
@@ -4292,7 +4355,7 @@
         <v>dev</v>
       </c>
       <c r="D61" s="13">
-        <f t="shared" ref="D61" si="6">D55</f>
+        <f t="shared" ref="D61" si="8">D55</f>
         <v>0</v>
       </c>
       <c r="E61" s="13">
@@ -4340,11 +4403,11 @@
     <row r="62" spans="2:18">
       <c r="B62" s="4"/>
       <c r="C62" s="5" t="str">
-        <f t="shared" ref="C62:D63" si="7">C56</f>
+        <f t="shared" ref="C62:D63" si="9">C56</f>
         <v>test</v>
       </c>
       <c r="D62" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7200</v>
       </c>
       <c r="E62" s="13">
@@ -4392,11 +4455,11 @@
     <row r="63" spans="2:18">
       <c r="B63" s="4"/>
       <c r="C63" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>prod</v>
       </c>
       <c r="D63" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>946560</v>
       </c>
       <c r="E63" s="13">
@@ -4642,7 +4705,7 @@
     <row r="70" spans="2:18">
       <c r="B70" s="4"/>
       <c r="C70" s="5" t="str">
-        <f t="shared" ref="C70:C71" si="8">C62</f>
+        <f t="shared" ref="C70:C71" si="10">C62</f>
         <v>test</v>
       </c>
       <c r="E70" s="22">
@@ -4683,7 +4746,7 @@
     <row r="71" spans="2:18">
       <c r="B71" s="4"/>
       <c r="C71" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>prod</v>
       </c>
       <c r="E71" s="22">
@@ -4710,7 +4773,7 @@
       <c r="K71" s="35"/>
       <c r="L71" s="24"/>
       <c r="M71" s="4"/>
-      <c r="N71" s="50"/>
+      <c r="N71" s="42"/>
       <c r="O71" s="6"/>
       <c r="Q71" s="50"/>
       <c r="R71" s="6"/>
@@ -4736,40 +4799,189 @@
       <c r="K72" s="36"/>
       <c r="L72" s="23"/>
       <c r="M72" s="4"/>
-      <c r="N72" s="50"/>
+      <c r="N72" s="42"/>
       <c r="O72" s="6"/>
       <c r="Q72" s="50"/>
       <c r="R72" s="6"/>
     </row>
     <row r="73" spans="2:18">
-      <c r="B73" s="4"/>
-      <c r="K73" s="6"/>
-      <c r="M73" s="15"/>
-      <c r="N73" s="51"/>
-      <c r="O73" s="11"/>
-      <c r="P73" s="10"/>
-      <c r="Q73" s="51"/>
-      <c r="R73" s="11"/>
-    </row>
-    <row r="74" spans="2:18" s="8" customFormat="1">
-      <c r="B74" s="17" t="s">
+      <c r="B73" s="7"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="36"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="42"/>
+      <c r="O73" s="6"/>
+      <c r="Q73" s="50"/>
+      <c r="R73" s="6"/>
+    </row>
+    <row r="74" spans="2:18">
+      <c r="B74" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H74" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J74" s="23"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="23"/>
+      <c r="M74" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="N74" s="42"/>
+      <c r="O74" s="6"/>
+      <c r="Q74" s="50"/>
+      <c r="R74" s="6"/>
+    </row>
+    <row r="75" spans="2:18">
+      <c r="B75" s="59"/>
+      <c r="C75" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="60">
+        <f>D56</f>
+        <v>7200</v>
+      </c>
+      <c r="E75" s="60">
+        <f>D75*30</f>
+        <v>216000</v>
+      </c>
+      <c r="F75" s="21"/>
+      <c r="G75" s="61">
+        <f>E75*$N$75/1000000</f>
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="H75" s="63">
+        <f>E75*$Q$31/1000*$N$76</f>
+        <v>19.439999999999998</v>
+      </c>
+      <c r="I75" s="61"/>
+      <c r="J75" s="61"/>
+      <c r="K75" s="62"/>
+      <c r="L75" s="23"/>
+      <c r="M75" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N75" s="45">
+        <v>3.5</v>
+      </c>
+      <c r="O75" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q75" s="50"/>
+      <c r="R75" s="6"/>
+    </row>
+    <row r="76" spans="2:18">
+      <c r="B76" s="59"/>
+      <c r="C76" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="60">
+        <f>D57</f>
+        <v>946560</v>
+      </c>
+      <c r="E76" s="60">
+        <f>D76*30</f>
+        <v>28396800</v>
+      </c>
+      <c r="F76" s="21"/>
+      <c r="G76" s="61">
+        <f>E76*$N$75/1000000</f>
+        <v>99.388800000000003</v>
+      </c>
+      <c r="H76" s="63">
+        <f>E76*$Q$31/1000*$N$76</f>
+        <v>2555.712</v>
+      </c>
+      <c r="I76" s="61"/>
+      <c r="J76" s="61"/>
+      <c r="K76" s="62"/>
+      <c r="L76" s="23"/>
+      <c r="M76" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="N76" s="45">
+        <v>0.09</v>
+      </c>
+      <c r="O76" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q76" s="50"/>
+      <c r="R76" s="6"/>
+    </row>
+    <row r="77" spans="2:18">
+      <c r="B77" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="G77" s="23">
+        <f>SUM(G75:G76)</f>
+        <v>100.1448</v>
+      </c>
+      <c r="H77" s="23">
+        <f>SUM(H75:H76)</f>
+        <v>2575.152</v>
+      </c>
+      <c r="I77" s="23"/>
+      <c r="J77" s="23"/>
+      <c r="K77" s="36"/>
+      <c r="L77" s="23"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="50"/>
+      <c r="O77" s="6"/>
+      <c r="Q77" s="50"/>
+      <c r="R77" s="6"/>
+    </row>
+    <row r="78" spans="2:18">
+      <c r="B78" s="4"/>
+      <c r="K78" s="6"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="51"/>
+      <c r="O78" s="11"/>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="51"/>
+      <c r="R78" s="11"/>
+    </row>
+    <row r="79" spans="2:18" s="8" customFormat="1">
+      <c r="B79" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="29">
-        <f>I65+J65+H58+H52+I72+J72</f>
-        <v>179303.29907887179</v>
-      </c>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="20"/>
-    </row>
-    <row r="77" spans="2:18" s="8" customFormat="1">
-      <c r="B77" s="8" t="s">
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="29">
+        <f>I65+J65+H58+H52+I72+J72+G77+H77</f>
+        <v>181978.5958788718</v>
+      </c>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="20"/>
+    </row>
+    <row r="82" spans="2:2" s="8" customFormat="1">
+      <c r="B82" s="8" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
comment out unneeded crap in node
</commit_message>
<xml_diff>
--- a/api-lambda-mock/ec2-vs-lambda.xlsx
+++ b/api-lambda-mock/ec2-vs-lambda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="31660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="31660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple EC2-vs-Lambda" sheetId="1" r:id="rId1"/>
@@ -1506,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P35" sqref="P35:P37"/>
     </sheetView>
   </sheetViews>
@@ -3105,7 +3105,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3380,11 +3382,11 @@
       </c>
       <c r="G12" s="39">
         <f t="shared" ref="G12:G21" si="3">VLOOKUP(D12,$M$30:$N$57,2,FALSE)</f>
-        <v>0.24440000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" ref="H12:H21" si="4">30*24*G12*F12</f>
-        <v>351.93600000000004</v>
+        <v>936</v>
       </c>
       <c r="I12" s="6"/>
       <c r="M12" s="55"/>
@@ -3409,11 +3411,11 @@
       </c>
       <c r="G13" s="39">
         <f t="shared" si="3"/>
-        <v>0.25769999999999998</v>
+        <v>0.30659999999999998</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="4"/>
-        <v>2040.9839999999999</v>
+        <v>2428.2719999999999</v>
       </c>
       <c r="I13" s="6"/>
       <c r="M13" s="55"/>
@@ -3438,11 +3440,11 @@
       </c>
       <c r="G14" s="39">
         <f t="shared" si="3"/>
-        <v>1.6899999999999998E-2</v>
+        <v>1.84E-2</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="4"/>
-        <v>24.335999999999999</v>
+        <v>26.495999999999999</v>
       </c>
       <c r="I14" s="6"/>
       <c r="M14" s="55"/>
@@ -3467,11 +3469,11 @@
       </c>
       <c r="G15" s="39">
         <f t="shared" si="3"/>
-        <v>1.111E-2</v>
+        <v>1.15E-2</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" si="4"/>
-        <v>87.991200000000006</v>
+        <v>91.08</v>
       </c>
       <c r="I15" s="6"/>
       <c r="M15" s="55"/>
@@ -3525,11 +3527,11 @@
       </c>
       <c r="G17" s="39">
         <f t="shared" si="3"/>
-        <v>4.1599999999999998E-2</v>
+        <v>4.6899999999999997E-2</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" si="4"/>
-        <v>449.28</v>
+        <v>506.52</v>
       </c>
       <c r="I17" s="6"/>
       <c r="M17" s="55"/>
@@ -3554,11 +3556,11 @@
       </c>
       <c r="G18" s="39">
         <f t="shared" si="3"/>
-        <v>7.6999999999999999E-2</v>
+        <v>9.6100000000000005E-2</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" si="4"/>
-        <v>277.2</v>
+        <v>345.96000000000004</v>
       </c>
       <c r="I18" s="6"/>
       <c r="M18" s="55"/>
@@ -3791,7 +3793,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="12">
         <f>SUM(H6:H26)</f>
-        <v>180413.14319999999</v>
+        <v>181515.74400000001</v>
       </c>
       <c r="I27" s="6"/>
       <c r="M27" s="4"/>
@@ -3862,10 +3864,10 @@
       </c>
       <c r="I30" s="6"/>
       <c r="M30" s="4" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="N30" s="43">
-        <v>7.6999999999999999E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="O30" s="6" t="s">
         <v>5</v>
@@ -3906,11 +3908,11 @@
         <v>0.63892800000000005</v>
       </c>
       <c r="I31" s="6"/>
-      <c r="M31" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="N31" s="43">
-        <v>0.83799999999999997</v>
+      <c r="M31" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="N31" s="44">
+        <v>0.42</v>
       </c>
       <c r="O31" s="6" t="s">
         <v>5</v>
@@ -3951,11 +3953,11 @@
         <v>83.997734399999999</v>
       </c>
       <c r="I32" s="6"/>
-      <c r="M32" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="N32" s="43">
-        <v>6.4999999999999997E-3</v>
+      <c r="M32" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="N32" s="44">
+        <v>0.84</v>
       </c>
       <c r="O32" s="6" t="s">
         <v>5</v>
@@ -3977,11 +3979,11 @@
         <v>84.636662400000006</v>
       </c>
       <c r="I33" s="6"/>
-      <c r="M33" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="N33" s="43">
-        <v>7.1000000000000004E-3</v>
+      <c r="M33" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="N33" s="44">
+        <v>1.68</v>
       </c>
       <c r="O33" s="6" t="s">
         <v>5</v>
@@ -3992,11 +3994,11 @@
     <row r="34" spans="2:18">
       <c r="B34" s="4"/>
       <c r="I34" s="6"/>
-      <c r="M34" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="N34" s="43">
-        <v>1.111E-2</v>
+      <c r="M34" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="N34" s="44">
+        <v>0.105</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>5</v>
@@ -4015,14 +4017,14 @@
       <c r="G35" s="18"/>
       <c r="H35" s="19">
         <f>H33+H27</f>
-        <v>180497.7798624</v>
+        <v>181600.38066240001</v>
       </c>
       <c r="I35" s="20"/>
-      <c r="M35" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="N35" s="43">
-        <v>1.2999999999999999E-2</v>
+      <c r="M35" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="N35" s="44">
+        <v>0.21</v>
       </c>
       <c r="O35" s="6" t="s">
         <v>5</v>
@@ -4033,10 +4035,10 @@
     <row r="36" spans="2:18" s="8" customFormat="1">
       <c r="H36" s="23"/>
       <c r="M36" s="4" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="N36" s="43">
-        <v>1.6199999999999999E-2</v>
+        <v>0.83799999999999997</v>
       </c>
       <c r="O36" s="6" t="s">
         <v>5</v>
@@ -4047,10 +4049,10 @@
     <row r="37" spans="2:18" s="8" customFormat="1">
       <c r="H37" s="23"/>
       <c r="M37" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N37" s="43">
-        <v>1.6899999999999998E-2</v>
+        <v>0.65</v>
       </c>
       <c r="O37" s="6" t="s">
         <v>5</v>
@@ -4061,10 +4063,10 @@
     <row r="38" spans="2:18" s="8" customFormat="1">
       <c r="H38" s="23"/>
       <c r="M38" s="4" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="N38" s="43">
-        <v>2.5999999999999999E-2</v>
+        <v>0.30659999999999998</v>
       </c>
       <c r="O38" s="6" t="s">
         <v>5</v>
@@ -4075,10 +4077,10 @@
     <row r="39" spans="2:18" s="8" customFormat="1">
       <c r="H39" s="23"/>
       <c r="M39" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N39" s="43">
-        <v>4.1599999999999998E-2</v>
+        <v>1.84E-2</v>
       </c>
       <c r="O39" s="6" t="s">
         <v>5</v>
@@ -4089,10 +4091,10 @@
     <row r="40" spans="2:18" s="8" customFormat="1">
       <c r="H40" s="23"/>
       <c r="M40" s="4" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="N40" s="43">
-        <v>5.1999999999999998E-2</v>
+        <v>1.15E-2</v>
       </c>
       <c r="O40" s="6" t="s">
         <v>5</v>
@@ -4103,10 +4105,10 @@
     <row r="41" spans="2:18" s="8" customFormat="1">
       <c r="H41" s="23"/>
       <c r="M41" s="4" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="N41" s="43">
-        <v>6.7000000000000004E-2</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="O41" s="6" t="s">
         <v>5</v>
@@ -4117,10 +4119,10 @@
     <row r="42" spans="2:18" s="8" customFormat="1">
       <c r="H42" s="23"/>
       <c r="M42" s="4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="N42" s="43">
-        <v>0.104</v>
+        <v>4.6899999999999997E-2</v>
       </c>
       <c r="O42" s="6" t="s">
         <v>5</v>
@@ -4130,11 +4132,11 @@
     </row>
     <row r="43" spans="2:18" s="8" customFormat="1">
       <c r="H43" s="23"/>
-      <c r="M43" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="N43" s="44">
-        <v>0.105</v>
+      <c r="M43" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N43" s="43">
+        <v>9.6100000000000005E-2</v>
       </c>
       <c r="O43" s="6" t="s">
         <v>5</v>
@@ -4145,10 +4147,10 @@
     <row r="44" spans="2:18" s="8" customFormat="1">
       <c r="H44" s="23"/>
       <c r="M44" s="4" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="N44" s="43">
-        <v>0.12</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="O44" s="6" t="s">
         <v>5</v>
@@ -4182,11 +4184,11 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="3"/>
-      <c r="M46" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="N46" s="44">
-        <v>0.21</v>
+      <c r="M46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" s="43">
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="O46" s="6" t="s">
         <v>5</v>
@@ -4198,10 +4200,10 @@
       <c r="B47" s="4"/>
       <c r="K47" s="6"/>
       <c r="M47" s="4" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="N47" s="43">
-        <v>0.23899999999999999</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="O47" s="6" t="s">
         <v>5</v>
@@ -4229,10 +4231,10 @@
       </c>
       <c r="K48" s="6"/>
       <c r="M48" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="N48" s="43">
-        <v>0.24440000000000001</v>
+        <v>2.3940000000000001</v>
       </c>
       <c r="O48" s="6" t="s">
         <v>5</v>
@@ -4259,10 +4261,10 @@
       </c>
       <c r="K49" s="6"/>
       <c r="M49" s="4" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="N49" s="43">
-        <v>0.25769999999999998</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="O49" s="6" t="s">
         <v>5</v>
@@ -4289,10 +4291,10 @@
       </c>
       <c r="K50" s="6"/>
       <c r="M50" s="4" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="N50" s="43">
-        <v>0.26600000000000001</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="O50" s="6" t="s">
         <v>5</v>
@@ -4311,18 +4313,18 @@
       <c r="F51" s="21"/>
       <c r="G51" s="39">
         <f>VLOOKUP(D51,$M$30:$N$57,2,FALSE)</f>
-        <v>0.25769999999999998</v>
+        <v>0.30659999999999998</v>
       </c>
       <c r="H51" s="9">
         <f>30*24*G51*E51</f>
-        <v>2040.9839999999999</v>
+        <v>2428.2719999999999</v>
       </c>
       <c r="K51" s="6"/>
-      <c r="M51" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="N51" s="44">
-        <v>0.42</v>
+      <c r="M51" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N51" s="43">
+        <v>0.12</v>
       </c>
       <c r="O51" s="6" t="s">
         <v>5</v>
@@ -4341,14 +4343,14 @@
       <c r="G52" s="8"/>
       <c r="H52" s="12">
         <f>SUM(H49:H51)</f>
-        <v>9233.7839999999997</v>
+        <v>9621.0720000000001</v>
       </c>
       <c r="K52" s="6"/>
       <c r="M52" s="4" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="N52" s="43">
-        <v>0.47899999999999998</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="O52" s="6" t="s">
         <v>5</v>
@@ -4360,10 +4362,10 @@
       <c r="B53" s="4"/>
       <c r="K53" s="6"/>
       <c r="M53" s="4" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="N53" s="43">
-        <v>0.53200000000000003</v>
+        <v>0.104</v>
       </c>
       <c r="O53" s="6" t="s">
         <v>5</v>
@@ -4396,11 +4398,11 @@
       </c>
       <c r="I54" s="8"/>
       <c r="K54" s="6"/>
-      <c r="M54" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="N54" s="44">
-        <v>0.84</v>
+      <c r="M54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N54" s="43">
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="O54" s="6" t="s">
         <v>5</v>
@@ -4409,7 +4411,7 @@
         <v>60</v>
       </c>
       <c r="Q54" s="42">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="R54" s="6" t="s">
         <v>61</v>
@@ -4440,10 +4442,10 @@
       </c>
       <c r="K55" s="6"/>
       <c r="M55" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N55" s="43">
-        <v>0.95799999999999996</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="O55" s="6" t="s">
         <v>5</v>
@@ -4463,23 +4465,23 @@
       </c>
       <c r="E56" s="13">
         <f>E31*$Q$54</f>
-        <v>44292857.142857149</v>
+        <v>4921428.5714285718</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="13">
         <f>(E56+D56)*30</f>
-        <v>1329001714.2857144</v>
+        <v>147858857.14285716</v>
       </c>
       <c r="H56" s="9">
         <f>D56*($Q$31/1000)*$N$26</f>
         <v>0.63892800000000005</v>
       </c>
       <c r="K56" s="6"/>
-      <c r="M56" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="N56" s="44">
-        <v>1.68</v>
+      <c r="M56" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N56" s="43">
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="O56" s="6" t="s">
         <v>5</v>
@@ -4499,12 +4501,12 @@
       </c>
       <c r="E57" s="13">
         <f>E32*$Q$54</f>
-        <v>835714285.71428561</v>
+        <v>92857142.857142851</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="13">
         <f>(E57+D57)*30</f>
-        <v>25099825371.42857</v>
+        <v>2814111085.7142854</v>
       </c>
       <c r="H57" s="9">
         <f>D57*($Q$31/1000)*$N$26</f>
@@ -4512,10 +4514,10 @@
       </c>
       <c r="K57" s="6"/>
       <c r="M57" s="4" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="N57" s="43">
-        <v>2.3940000000000001</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="O57" s="6" t="s">
         <v>5</v>
@@ -4651,7 +4653,7 @@
         <v>118</v>
       </c>
       <c r="Q61" s="42">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="R61" s="6" t="s">
         <v>121</v>
@@ -4669,24 +4671,24 @@
       </c>
       <c r="E62" s="13">
         <f>E56</f>
-        <v>44292857.142857149</v>
+        <v>4921428.5714285718</v>
       </c>
       <c r="F62" s="13"/>
       <c r="G62" s="13">
         <f>30*(E62+D62)</f>
-        <v>1329001714.2857144</v>
+        <v>147858857.14285716</v>
       </c>
       <c r="H62" s="13">
         <f>((D62+(E62*(1-$Q$61-$Q$65)))*30*($Q$59/1000)*($Q$58/1000))+           ((E62*$Q$61)*30*($Q$62/1000)*($Q$63/1000))+           ((E62*$Q$65)*30*($Q$66/1000)*($Q$67/1000))</f>
-        <v>442162911.0857144</v>
+        <v>70683088.45714286</v>
       </c>
       <c r="I62" s="9">
         <f>(G62/1000000)*$N$60</f>
-        <v>265.80034285714288</v>
+        <v>29.571771428571438</v>
       </c>
       <c r="J62" s="24">
         <f>H62*$N$61</f>
-        <v>7370.8557277988593</v>
+        <v>1178.2870845805717</v>
       </c>
       <c r="K62" s="35"/>
       <c r="L62" s="24"/>
@@ -4721,24 +4723,24 @@
       </c>
       <c r="E63" s="13">
         <f>E57</f>
-        <v>835714285.71428561</v>
+        <v>92857142.857142851</v>
       </c>
       <c r="F63" s="13"/>
       <c r="G63" s="13">
         <f>30*(E63+D63)</f>
-        <v>25099825371.42857</v>
+        <v>2814111085.7142854</v>
       </c>
       <c r="H63" s="13">
         <f>((D63+(E63*(1-$Q$61-$Q$65)))*30*($Q$59/1000)*($Q$58/1000))+           ((E63*$Q$61)*30*($Q$62/1000)*($Q$63/1000))+           ((E63*$Q$65)*30*($Q$66/1000)*($Q$67/1000))</f>
-        <v>8343941687.5885715</v>
+        <v>1334888430.4457142</v>
       </c>
       <c r="I63" s="9">
         <f>(G63/1000000)*$N$60</f>
-        <v>5019.9650742857148</v>
+        <v>562.82221714285708</v>
       </c>
       <c r="J63" s="24">
         <f>H63*$N$61</f>
-        <v>139093.50793210149</v>
+        <v>22252.590135530059</v>
       </c>
       <c r="K63" s="35"/>
       <c r="L63" s="24"/>
@@ -4770,19 +4772,19 @@
       <c r="F64" s="13"/>
       <c r="G64" s="13">
         <f>SUM(G61:G63)</f>
-        <v>26428827085.714283</v>
+        <v>2961969942.8571424</v>
       </c>
       <c r="H64" s="13">
         <f>SUM(H61:H63)</f>
-        <v>8786104598.6742859</v>
+        <v>1405571518.9028571</v>
       </c>
       <c r="I64" s="9">
         <f>(G64/1000000)*$N$60</f>
-        <v>5285.7654171428567</v>
+        <v>592.39398857142851</v>
       </c>
       <c r="J64" s="24">
         <f>H64*$N$61</f>
-        <v>146464.36365990035</v>
+        <v>23430.877220110629</v>
       </c>
       <c r="K64" s="35"/>
       <c r="L64" s="24"/>
@@ -4802,19 +4804,19 @@
       <c r="F65" s="27"/>
       <c r="G65" s="27">
         <f>IF(G64&gt;N62,G64-N62,0)</f>
-        <v>26427827085.714283</v>
+        <v>2960969942.8571424</v>
       </c>
       <c r="H65" s="27">
         <f>IF(H64&gt;N63,H64-N63,0)</f>
-        <v>8784504598.6742859</v>
+        <v>1403971518.9028571</v>
       </c>
       <c r="I65" s="12">
         <f>(G65/1000000)*$N$60</f>
-        <v>5285.5654171428569</v>
+        <v>592.19398857142858</v>
       </c>
       <c r="J65" s="23">
         <f>H65*$N$61</f>
-        <v>146437.69165990036</v>
+        <v>23404.205220110631</v>
       </c>
       <c r="K65" s="36"/>
       <c r="L65" s="23"/>
@@ -4967,12 +4969,12 @@
       </c>
       <c r="E70" s="22">
         <f>E62+D62</f>
-        <v>44300057.142857149</v>
+        <v>4928628.5714285718</v>
       </c>
       <c r="F70" s="22"/>
       <c r="G70" s="22">
         <f>E70*30</f>
-        <v>1329001714.2857144</v>
+        <v>147858857.14285716</v>
       </c>
       <c r="H70" s="5">
         <f>IF(E70 &gt; 0,IF(E70 &lt;(24*60*60)*1000,24,E70/60/60/1000)*$Q$69,0)</f>
@@ -4980,7 +4982,7 @@
       </c>
       <c r="I70" s="24">
         <f>G70/100000*$N$68*($Q$31/$N$70)</f>
-        <v>744.24095999999997</v>
+        <v>82.800960000000018</v>
       </c>
       <c r="J70" s="24">
         <f>H70*$N$69*30</f>
@@ -5008,24 +5010,24 @@
       </c>
       <c r="E71" s="22">
         <f>E63+D63</f>
-        <v>836660845.71428561</v>
+        <v>93803702.857142851</v>
       </c>
       <c r="F71" s="22"/>
       <c r="G71" s="22">
         <f>E71*30</f>
-        <v>25099825371.42857</v>
+        <v>2814111085.7142854</v>
       </c>
       <c r="H71" s="57">
         <f>IF(E71 &gt; 0,IF(E71 &lt;(24*60*60)*1000,24,E71/60/60/1000)*$Q$69,0)</f>
-        <v>6972.1737142857137</v>
+        <v>781.69752380952377</v>
       </c>
       <c r="I71" s="24">
         <f>G71/100000*$N$68*($Q$31/$N$70)</f>
-        <v>14055.902208</v>
+        <v>1575.9022079999997</v>
       </c>
       <c r="J71" s="24">
         <f>H71*$N$69*30</f>
-        <v>3137.4781714285709</v>
+        <v>351.76388571428572</v>
       </c>
       <c r="K71" s="35"/>
       <c r="L71" s="24"/>
@@ -5047,11 +5049,11 @@
       <c r="H72" s="8"/>
       <c r="I72" s="23">
         <f>SUM(I69:I71)</f>
-        <v>14800.143167999999</v>
+        <v>1658.7031679999998</v>
       </c>
       <c r="J72" s="23">
         <f>SUM(J69:J71)</f>
-        <v>3461.4781714285709</v>
+        <v>675.76388571428561</v>
       </c>
       <c r="K72" s="36"/>
       <c r="L72" s="23"/>
@@ -5274,7 +5276,7 @@
       <c r="G80" s="18"/>
       <c r="H80" s="29">
         <f>I65+J65+H58+H52+I72+J72+G78+H78</f>
-        <v>181978.5958788718</v>
+        <v>38711.87172479635</v>
       </c>
       <c r="I80" s="18"/>
       <c r="J80" s="18"/>
@@ -5286,9 +5288,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <sortState ref="D7:E23">
-    <sortCondition ref="D6"/>
+  <sortState ref="M30:N57">
+    <sortCondition ref="M30:M57"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
minor cosmetic changes to spreadsheet
</commit_message>
<xml_diff>
--- a/api-lambda-mock/ec2-vs-lambda.xlsx
+++ b/api-lambda-mock/ec2-vs-lambda.xlsx
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="138">
   <si>
     <t>AWS EC2 costs for a small SOA architecture</t>
   </si>
@@ -485,9 +485,6 @@
     <t>YOU DON'T REALLY WANT TO EDIT PRICING</t>
   </si>
   <si>
-    <t>BECAUSE IT'S SET BY AWS/AZURE/WHOEVER</t>
-  </si>
-  <si>
     <t>med %</t>
   </si>
   <si>
@@ -534,14 +531,30 @@
   </si>
   <si>
     <t>Call Per Month</t>
+  </si>
+  <si>
+    <t>msgs/sec</t>
+  </si>
+  <si>
+    <t>BECAUSE IT'S SET BY AWS</t>
+  </si>
+  <si>
+    <t>THESE THINGS VARY BY APPLICATION STACK</t>
+  </si>
+  <si>
+    <t>YOU SHOULD UNDERSTAND AND CHANGE</t>
+  </si>
+  <si>
+    <t>ALL OF THESE VALUES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -746,7 +759,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="164">
+  <cellStyleXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -911,8 +924,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1007,11 +1044,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="164">
+  <cellStyles count="188">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1094,6 +1134,18 @@
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1175,6 +1227,18 @@
     <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2535,7 +2599,7 @@
         <v>64</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q35" s="42">
         <v>0.5</v>
@@ -2587,7 +2651,7 @@
         <v>66</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q36" s="42">
         <v>1000</v>
@@ -2625,7 +2689,7 @@
       <c r="N37" s="46"/>
       <c r="O37" s="6"/>
       <c r="P37" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q37" s="42">
         <v>512</v>
@@ -2884,30 +2948,30 @@
     </row>
     <row r="46" spans="2:18">
       <c r="B46" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="F46" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I46" s="23"/>
       <c r="J46" s="23"/>
       <c r="K46" s="36"/>
       <c r="L46" s="23"/>
       <c r="M46" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N46" s="42"/>
       <c r="O46" s="6"/>
@@ -2944,7 +3008,7 @@
       <c r="K47" s="62"/>
       <c r="L47" s="23"/>
       <c r="M47" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N47" s="45">
         <v>3.5</v>
@@ -2985,13 +3049,13 @@
       <c r="K48" s="62"/>
       <c r="L48" s="23"/>
       <c r="M48" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N48" s="45">
         <v>0.09</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q48" s="50"/>
       <c r="R48" s="6"/>
@@ -3033,7 +3097,7 @@
     </row>
     <row r="50" spans="2:18">
       <c r="B50" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -3106,24 +3170,28 @@
   <dimension ref="B2:R83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="5"/>
-    <col min="4" max="4" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="5"/>
-    <col min="10" max="10" width="15.33203125" style="5" customWidth="1"/>
-    <col min="11" max="12" width="11.1640625" style="5" customWidth="1"/>
-    <col min="13" max="14" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="3.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="5"/>
+    <col min="4" max="4" width="12.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" style="5" customWidth="1"/>
     <col min="15" max="15" width="12.5" style="5" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.5" style="5" customWidth="1"/>
     <col min="19" max="16384" width="10.83203125" style="5"/>
   </cols>
@@ -3174,18 +3242,18 @@
         <v>6</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="49"/>
-      <c r="O5" s="3" t="s">
+      <c r="N5" s="68"/>
+      <c r="O5" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="3" t="s">
+      <c r="Q5" s="68"/>
+      <c r="R5" s="53" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3211,9 +3279,7 @@
         <v>58.32</v>
       </c>
       <c r="I6" s="6"/>
-      <c r="M6" s="58" t="s">
-        <v>116</v>
-      </c>
+      <c r="M6" s="58"/>
       <c r="N6" s="56"/>
       <c r="O6" s="32"/>
       <c r="P6" s="8"/>
@@ -3242,8 +3308,8 @@
         <v>12700.8</v>
       </c>
       <c r="I7" s="6"/>
-      <c r="M7" s="58" t="s">
-        <v>117</v>
+      <c r="M7" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="N7" s="56"/>
       <c r="O7" s="32"/>
@@ -3273,7 +3339,9 @@
         <v>74995.199999999997</v>
       </c>
       <c r="I8" s="6"/>
-      <c r="M8" s="55"/>
+      <c r="M8" s="55" t="s">
+        <v>134</v>
+      </c>
       <c r="N8" s="56"/>
       <c r="O8" s="32"/>
       <c r="P8" s="8"/>
@@ -3624,7 +3692,9 @@
       <c r="M20" s="55"/>
       <c r="N20" s="56"/>
       <c r="O20" s="32"/>
-      <c r="P20" s="8"/>
+      <c r="P20" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="Q20" s="56"/>
       <c r="R20" s="32"/>
     </row>
@@ -3653,7 +3723,9 @@
       <c r="M21" s="55"/>
       <c r="N21" s="56"/>
       <c r="O21" s="32"/>
-      <c r="P21" s="8"/>
+      <c r="P21" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="Q21" s="56"/>
       <c r="R21" s="32"/>
     </row>
@@ -3682,7 +3754,9 @@
       <c r="M22" s="55"/>
       <c r="N22" s="56"/>
       <c r="O22" s="32"/>
-      <c r="P22" s="8"/>
+      <c r="P22" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="Q22" s="56"/>
       <c r="R22" s="32"/>
     </row>
@@ -4411,7 +4485,7 @@
         <v>60</v>
       </c>
       <c r="Q54" s="42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R54" s="6" t="s">
         <v>61</v>
@@ -4465,12 +4539,12 @@
       </c>
       <c r="E56" s="13">
         <f>E31*$Q$54</f>
-        <v>4921428.5714285718</v>
+        <v>24607142.857142858</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="13">
         <f>(E56+D56)*30</f>
-        <v>147858857.14285716</v>
+        <v>738430285.71428573</v>
       </c>
       <c r="H56" s="9">
         <f>D56*($Q$31/1000)*$N$26</f>
@@ -4501,12 +4575,12 @@
       </c>
       <c r="E57" s="13">
         <f>E32*$Q$54</f>
-        <v>92857142.857142851</v>
+        <v>464285714.28571427</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="13">
         <f>(E57+D57)*30</f>
-        <v>2814111085.7142854</v>
+        <v>13956968228.571428</v>
       </c>
       <c r="H57" s="9">
         <f>D57*($Q$31/1000)*$N$26</f>
@@ -4606,6 +4680,8 @@
       <c r="O60" s="6" t="s">
         <v>65</v>
       </c>
+      <c r="Q60" s="42"/>
+      <c r="R60" s="6"/>
     </row>
     <row r="61" spans="2:18">
       <c r="B61" s="4"/>
@@ -4650,13 +4726,13 @@
         <v>65</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q61" s="42">
         <v>0.25</v>
       </c>
       <c r="R61" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="2:18">
@@ -4671,24 +4747,24 @@
       </c>
       <c r="E62" s="13">
         <f>E56</f>
-        <v>4921428.5714285718</v>
+        <v>24607142.857142858</v>
       </c>
       <c r="F62" s="13"/>
       <c r="G62" s="13">
         <f>30*(E62+D62)</f>
-        <v>147858857.14285716</v>
+        <v>738430285.71428573</v>
       </c>
       <c r="H62" s="13">
         <f>((D62+(E62*(1-$Q$61-$Q$65)))*30*($Q$59/1000)*($Q$58/1000))+           ((E62*$Q$61)*30*($Q$62/1000)*($Q$63/1000))+           ((E62*$Q$65)*30*($Q$66/1000)*($Q$67/1000))</f>
-        <v>70683088.45714286</v>
+        <v>489401066.05714291</v>
       </c>
       <c r="I62" s="9">
         <f>(G62/1000000)*$N$60</f>
-        <v>29.571771428571438</v>
+        <v>147.68605714285715</v>
       </c>
       <c r="J62" s="24">
         <f>H62*$N$61</f>
-        <v>1178.2870845805717</v>
+        <v>8158.3157711725726</v>
       </c>
       <c r="K62" s="35"/>
       <c r="L62" s="24"/>
@@ -4702,7 +4778,7 @@
         <v>64</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q62" s="46">
         <v>1000</v>
@@ -4723,24 +4799,24 @@
       </c>
       <c r="E63" s="13">
         <f>E57</f>
-        <v>92857142.857142851</v>
+        <v>464285714.28571427</v>
       </c>
       <c r="F63" s="13"/>
       <c r="G63" s="13">
         <f>30*(E63+D63)</f>
-        <v>2814111085.7142854</v>
+        <v>13956968228.571428</v>
       </c>
       <c r="H63" s="13">
         <f>((D63+(E63*(1-$Q$61-$Q$65)))*30*($Q$59/1000)*($Q$58/1000))+           ((E63*$Q$61)*30*($Q$62/1000)*($Q$63/1000))+           ((E63*$Q$65)*30*($Q$66/1000)*($Q$67/1000))</f>
-        <v>1334888430.4457142</v>
+        <v>9235227630.445715</v>
       </c>
       <c r="I63" s="9">
         <f>(G63/1000000)*$N$60</f>
-        <v>562.82221714285708</v>
+        <v>2791.3936457142859</v>
       </c>
       <c r="J63" s="24">
         <f>H63*$N$61</f>
-        <v>22252.590135530059</v>
+        <v>153951.2445995301</v>
       </c>
       <c r="K63" s="35"/>
       <c r="L63" s="24"/>
@@ -4754,7 +4830,7 @@
         <v>66</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q63" s="42">
         <v>1024</v>
@@ -4772,19 +4848,19 @@
       <c r="F64" s="13"/>
       <c r="G64" s="13">
         <f>SUM(G61:G63)</f>
-        <v>2961969942.8571424</v>
+        <v>14695398514.285713</v>
       </c>
       <c r="H64" s="13">
         <f>SUM(H61:H63)</f>
-        <v>1405571518.9028571</v>
+        <v>9724628696.5028572</v>
       </c>
       <c r="I64" s="9">
         <f>(G64/1000000)*$N$60</f>
-        <v>592.39398857142851</v>
+        <v>2939.0797028571428</v>
       </c>
       <c r="J64" s="24">
         <f>H64*$N$61</f>
-        <v>23430.877220110629</v>
+        <v>162109.56037070265</v>
       </c>
       <c r="K64" s="35"/>
       <c r="L64" s="24"/>
@@ -4804,19 +4880,19 @@
       <c r="F65" s="27"/>
       <c r="G65" s="27">
         <f>IF(G64&gt;N62,G64-N62,0)</f>
-        <v>2960969942.8571424</v>
+        <v>14694398514.285713</v>
       </c>
       <c r="H65" s="27">
         <f>IF(H64&gt;N63,H64-N63,0)</f>
-        <v>1403971518.9028571</v>
+        <v>9723028696.5028572</v>
       </c>
       <c r="I65" s="12">
         <f>(G65/1000000)*$N$60</f>
-        <v>592.19398857142858</v>
+        <v>2938.8797028571425</v>
       </c>
       <c r="J65" s="23">
         <f>H65*$N$61</f>
-        <v>23404.205220110631</v>
+        <v>162082.88837070265</v>
       </c>
       <c r="K65" s="36"/>
       <c r="L65" s="23"/>
@@ -4827,7 +4903,7 @@
         <v>37</v>
       </c>
       <c r="Q65" s="42">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="R65" s="6" t="s">
         <v>71</v>
@@ -4852,7 +4928,6 @@
         <v>73</v>
       </c>
       <c r="Q66" s="46">
-        <f>3*60*1000</f>
         <v>180000</v>
       </c>
       <c r="R66" s="6" t="s">
@@ -4886,7 +4961,9 @@
       <c r="E68" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F68" s="8"/>
+      <c r="F68" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="G68" s="8" t="s">
         <v>43</v>
       </c>
@@ -4899,7 +4976,9 @@
       <c r="J68" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="K68" s="37"/>
+      <c r="K68" s="37" t="s">
+        <v>133</v>
+      </c>
       <c r="L68" s="28"/>
       <c r="M68" s="33" t="s">
         <v>81</v>
@@ -4923,7 +5002,10 @@
         <f>E61+D61</f>
         <v>0</v>
       </c>
-      <c r="F69" s="22"/>
+      <c r="F69" s="22">
+        <f>H69/24</f>
+        <v>0</v>
+      </c>
       <c r="G69" s="22">
         <f>E69*30</f>
         <v>0</v>
@@ -4940,7 +5022,10 @@
         <f>H69*$N$69*30</f>
         <v>0</v>
       </c>
-      <c r="K69" s="35"/>
+      <c r="K69" s="66">
+        <f t="shared" ref="K69:K71" si="10">K61+J61</f>
+        <v>0</v>
+      </c>
       <c r="L69" s="24"/>
       <c r="M69" s="4" t="s">
         <v>47</v>
@@ -4964,17 +5049,20 @@
     <row r="70" spans="2:18">
       <c r="B70" s="4"/>
       <c r="C70" s="5" t="str">
-        <f t="shared" ref="C70:C71" si="10">C62</f>
+        <f t="shared" ref="C70:C71" si="11">C62</f>
         <v>test</v>
       </c>
       <c r="E70" s="22">
         <f>E62+D62</f>
-        <v>4928628.5714285718</v>
-      </c>
-      <c r="F70" s="22"/>
+        <v>24614342.857142858</v>
+      </c>
+      <c r="F70" s="22">
+        <f>H70/24</f>
+        <v>30</v>
+      </c>
       <c r="G70" s="22">
         <f>E70*30</f>
-        <v>147858857.14285716</v>
+        <v>738430285.71428573</v>
       </c>
       <c r="H70" s="5">
         <f>IF(E70 &gt; 0,IF(E70 &lt;(24*60*60)*1000,24,E70/60/60/1000)*$Q$69,0)</f>
@@ -4982,13 +5070,16 @@
       </c>
       <c r="I70" s="24">
         <f>G70/100000*$N$68*($Q$31/$N$70)</f>
-        <v>82.800960000000018</v>
+        <v>413.52096000000006</v>
       </c>
       <c r="J70" s="24">
         <f>H70*$N$69*30</f>
         <v>323.99999999999994</v>
       </c>
-      <c r="K70" s="35"/>
+      <c r="K70" s="66">
+        <f>E70/24/60/60</f>
+        <v>284.88822751322749</v>
+      </c>
       <c r="L70" s="24"/>
       <c r="M70" s="4" t="s">
         <v>85</v>
@@ -5005,36 +5096,42 @@
     <row r="71" spans="2:18">
       <c r="B71" s="4"/>
       <c r="C71" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>prod</v>
       </c>
       <c r="E71" s="22">
         <f>E63+D63</f>
-        <v>93803702.857142851</v>
-      </c>
-      <c r="F71" s="22"/>
+        <v>465232274.28571427</v>
+      </c>
+      <c r="F71" s="22">
+        <f>H71/24</f>
+        <v>161.53898412698413</v>
+      </c>
       <c r="G71" s="22">
         <f>E71*30</f>
-        <v>2814111085.7142854</v>
+        <v>13956968228.571428</v>
       </c>
       <c r="H71" s="57">
         <f>IF(E71 &gt; 0,IF(E71 &lt;(24*60*60)*1000,24,E71/60/60/1000)*$Q$69,0)</f>
-        <v>781.69752380952377</v>
+        <v>3876.9356190476192</v>
       </c>
       <c r="I71" s="24">
         <f>G71/100000*$N$68*($Q$31/$N$70)</f>
-        <v>1575.9022079999997</v>
+        <v>7815.9022080000004</v>
       </c>
       <c r="J71" s="24">
         <f>H71*$N$69*30</f>
-        <v>351.76388571428572</v>
-      </c>
-      <c r="K71" s="35"/>
+        <v>1744.6210285714287</v>
+      </c>
+      <c r="K71" s="66">
+        <f>E71/24/60/60</f>
+        <v>5384.6328042328041</v>
+      </c>
       <c r="L71" s="24"/>
       <c r="M71" s="4"/>
       <c r="N71" s="42"/>
       <c r="O71" s="6"/>
-      <c r="Q71" s="50"/>
+      <c r="Q71" s="42"/>
       <c r="R71" s="6"/>
     </row>
     <row r="72" spans="2:18">
@@ -5049,18 +5146,18 @@
       <c r="H72" s="8"/>
       <c r="I72" s="23">
         <f>SUM(I69:I71)</f>
-        <v>1658.7031679999998</v>
+        <v>8229.4231680000012</v>
       </c>
       <c r="J72" s="23">
         <f>SUM(J69:J71)</f>
-        <v>675.76388571428561</v>
-      </c>
-      <c r="K72" s="36"/>
+        <v>2068.6210285714287</v>
+      </c>
+      <c r="K72" s="65"/>
       <c r="L72" s="23"/>
       <c r="M72" s="4"/>
       <c r="N72" s="42"/>
       <c r="O72" s="6"/>
-      <c r="Q72" s="50"/>
+      <c r="Q72" s="42"/>
       <c r="R72" s="6"/>
     </row>
     <row r="73" spans="2:18">
@@ -5078,28 +5175,28 @@
       <c r="M73" s="4"/>
       <c r="N73" s="42"/>
       <c r="O73" s="6"/>
-      <c r="Q73" s="50"/>
+      <c r="Q73" s="42"/>
       <c r="R73" s="6"/>
     </row>
     <row r="74" spans="2:18">
       <c r="B74" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E74" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="F74" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I74" s="23"/>
       <c r="J74" s="23"/>
@@ -5108,7 +5205,7 @@
       <c r="M74" s="7"/>
       <c r="N74" s="42"/>
       <c r="O74" s="6"/>
-      <c r="Q74" s="50"/>
+      <c r="Q74" s="42"/>
       <c r="R74" s="6"/>
     </row>
     <row r="75" spans="2:18" s="21" customFormat="1">
@@ -5140,12 +5237,12 @@
       <c r="K75" s="62"/>
       <c r="L75" s="61"/>
       <c r="M75" s="59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N75" s="41"/>
       <c r="O75" s="64"/>
-      <c r="Q75" s="65"/>
-      <c r="R75" s="64"/>
+      <c r="Q75" s="42"/>
+      <c r="R75" s="6"/>
     </row>
     <row r="76" spans="2:18">
       <c r="B76" s="59"/>
@@ -5177,7 +5274,7 @@
       <c r="K76" s="62"/>
       <c r="L76" s="23"/>
       <c r="M76" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N76" s="45">
         <v>3.5</v>
@@ -5185,7 +5282,7 @@
       <c r="O76" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Q76" s="50"/>
+      <c r="Q76" s="42"/>
       <c r="R76" s="6"/>
     </row>
     <row r="77" spans="2:18">
@@ -5218,20 +5315,20 @@
       <c r="K77" s="62"/>
       <c r="L77" s="23"/>
       <c r="M77" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N77" s="45">
         <v>0.09</v>
       </c>
       <c r="O77" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q77" s="50"/>
+        <v>123</v>
+      </c>
+      <c r="Q77" s="42"/>
       <c r="R77" s="6"/>
     </row>
     <row r="78" spans="2:18">
       <c r="B78" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
@@ -5250,9 +5347,9 @@
       <c r="K78" s="36"/>
       <c r="L78" s="23"/>
       <c r="M78" s="4"/>
-      <c r="N78" s="50"/>
+      <c r="N78" s="42"/>
       <c r="O78" s="6"/>
-      <c r="Q78" s="50"/>
+      <c r="Q78" s="42"/>
       <c r="R78" s="6"/>
     </row>
     <row r="79" spans="2:18">
@@ -5276,7 +5373,7 @@
       <c r="G80" s="18"/>
       <c r="H80" s="29">
         <f>I65+J65+H58+H52+I72+J72+G78+H78</f>
-        <v>38711.87172479635</v>
+        <v>187700.81773253126</v>
       </c>
       <c r="I80" s="18"/>
       <c r="J80" s="18"/>

</xml_diff>